<commit_message>
Separate Gas and Liquid
Separate Gas and Liquid Phase from each other to prevent gas compounds to participate in diffusion and steady state checks.
Bug fixes
</commit_message>
<xml_diff>
--- a/planning/Templates/AF_template.xlsx
+++ b/planning/Templates/AF_template.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\tsbie\Documents\Universiteit\Master\Jaar 2\MEP\Code\IbM-Fermentation\IbM-Fermentation\planning\Templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C07007-BB1C-4B31-A7E2-FC27FF08F10E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E791C7C-27AF-4AA9-8FD0-B89CE37F9912}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="808" firstSheet="7" activeTab="9" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" tabRatio="808" firstSheet="3" activeTab="8" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Information" sheetId="30" r:id="rId1"/>
@@ -80,7 +80,6 @@
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>tc={0EA7B4BE-563B-4CD4-BC00-BD4C733C370E}</author>
-    <author>tc={AF29ABDE-2FE2-450D-BCB8-3B17CE2D1E3B}</author>
   </authors>
   <commentList>
     <comment ref="B4" authorId="0" shapeId="0" xr:uid="{0EA7B4BE-563B-4CD4-BC00-BD4C733C370E}">
@@ -89,14 +88,6 @@
 Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
 Comment:
     HCO3- Diffusivity</t>
-      </text>
-    </comment>
-    <comment ref="B8" authorId="1" shapeId="0" xr:uid="{AF29ABDE-2FE2-450D-BCB8-3B17CE2D1E3B}">
-      <text>
-        <t>[Threaded comment]
-Your version of Excel allows you to read this threaded comment; however, any edits to it will get removed if the file is opened in a newer version of Excel. Learn more: https://go.microsoft.com/fwlink/?linkid=870924
-Comment:
-    Gaseous CO2 diffusivity</t>
       </text>
     </comment>
   </commentList>
@@ -151,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C15" authorId="0" shapeId="0" xr:uid="{2BF6DF0C-A230-43E0-898A-E09FD5479204}">
+    <comment ref="C12" authorId="0" shapeId="0" xr:uid="{2BF6DF0C-A230-43E0-898A-E09FD5479204}">
       <text>
         <r>
           <rPr>
@@ -203,7 +194,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="707" uniqueCount="303">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="659" uniqueCount="302">
   <si>
     <t>AOB/AOA</t>
   </si>
@@ -1534,9 +1525,6 @@
   </si>
   <si>
     <t>eA</t>
-  </si>
-  <si>
-    <t>G</t>
   </si>
   <si>
     <t>Set the Henry coefficient if necessary and indicate whether the compound is not transfered to the gas phase (0), aquaous and leaving (-1) or gaseous and entering (1). Make sure that all compounds are in the same order and have the same name as in the rest of the Excel file</t>
@@ -1926,7 +1914,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="87">
+  <borders count="85">
     <border>
       <left/>
       <right/>
@@ -2935,17 +2923,6 @@
       <right style="thin">
         <color rgb="FFB2B2B2"/>
       </right>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -2967,19 +2944,6 @@
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -3052,7 +3016,7 @@
     <xf numFmtId="0" fontId="35" fillId="11" borderId="39" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="269">
+  <cellXfs count="265">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="7"/>
     <xf numFmtId="169" fontId="1" fillId="0" borderId="0" xfId="7" applyNumberFormat="1"/>
@@ -3424,9 +3388,6 @@
     <xf numFmtId="1" fontId="2" fillId="11" borderId="39" xfId="9" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="2" fillId="11" borderId="65" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="25" fillId="11" borderId="37" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3528,27 +3489,12 @@
     <xf numFmtId="0" fontId="2" fillId="11" borderId="79" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="52" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="77" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="54" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="11" borderId="80" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="54" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="11" borderId="81" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="11" borderId="82" xfId="9" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="36" fillId="0" borderId="30" xfId="10" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="14" xfId="10" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -3597,7 +3543,7 @@
     <xf numFmtId="0" fontId="36" fillId="0" borderId="15" xfId="10" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="11" fontId="36" fillId="0" borderId="83" xfId="10" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="36" fillId="0" borderId="81" xfId="10" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="16" xfId="10" applyBorder="1" applyAlignment="1">
@@ -3663,13 +3609,19 @@
     <xf numFmtId="0" fontId="0" fillId="11" borderId="51" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="11" borderId="85" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="2" fillId="11" borderId="83" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="2" fillId="11" borderId="82" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="11" fontId="2" fillId="11" borderId="84" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="11" fontId="2" fillId="11" borderId="86" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="11" fontId="0" fillId="11" borderId="50" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="11" fontId="25" fillId="11" borderId="56" xfId="9" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="12" xfId="7" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3726,7 +3678,7 @@
     <xf numFmtId="0" fontId="29" fillId="0" borderId="35" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="29" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="36" fillId="0" borderId="22" xfId="10" applyBorder="1" applyAlignment="1">
@@ -4326,9 +4278,6 @@
   <threadedComment ref="B4" dT="2024-05-03T14:34:30.91" personId="{AEEE75E0-0682-414F-A9ED-97F1D150B997}" id="{0EA7B4BE-563B-4CD4-BC00-BD4C733C370E}">
     <text>HCO3- Diffusivity</text>
   </threadedComment>
-  <threadedComment ref="B8" dT="2024-05-03T14:34:43.95" personId="{AEEE75E0-0682-414F-A9ED-97F1D150B997}" id="{AF29ABDE-2FE2-450D-BCB8-3B17CE2D1E3B}">
-    <text>Gaseous CO2 diffusivity</text>
-  </threadedComment>
 </ThreadedComments>
 </file>
 
@@ -4356,47 +4305,47 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:1" ht="21" x14ac:dyDescent="0.4">
-      <c r="A1" s="177" t="s">
+      <c r="A1" s="176" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A2" s="178" t="s">
+      <c r="A2" s="177" t="s">
         <v>239</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="27" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="176" t="s">
+      <c r="A3" s="175" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="175" t="s">
+      <c r="A4" s="174" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="28.8" x14ac:dyDescent="0.25">
-      <c r="A5" s="171" t="s">
+      <c r="A5" s="170" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A6" s="170" t="s">
+      <c r="A6" s="169" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A7" s="172" t="s">
+      <c r="A7" s="171" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="52.8" x14ac:dyDescent="0.25">
-      <c r="A8" s="173" t="s">
+      <c r="A8" s="172" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="40.200000000000003" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="174" t="s">
+      <c r="A9" s="173" t="s">
         <v>245</v>
       </c>
     </row>
@@ -4429,10 +4378,10 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4458,10 +4407,10 @@
       <c r="D1" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="E1" s="260" t="s">
+      <c r="E1" s="256" t="s">
         <v>209</v>
       </c>
-      <c r="F1" s="231"/>
+      <c r="F1" s="225"/>
       <c r="G1" s="69"/>
       <c r="H1" s="69"/>
       <c r="I1" s="69"/>
@@ -4480,8 +4429,8 @@
       <c r="D2" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="260"/>
-      <c r="F2" s="231"/>
+      <c r="E2" s="256"/>
+      <c r="F2" s="225"/>
       <c r="G2" s="69"/>
       <c r="H2" s="69"/>
       <c r="I2" s="69"/>
@@ -4500,8 +4449,8 @@
       <c r="D3" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="E3" s="260"/>
-      <c r="F3" s="231"/>
+      <c r="E3" s="256"/>
+      <c r="F3" s="225"/>
       <c r="G3" s="69"/>
       <c r="H3" s="69"/>
       <c r="I3" s="69"/>
@@ -4512,7 +4461,7 @@
         <v>76</v>
       </c>
       <c r="B4" s="121">
-        <v>9.9999999999999995E-21</v>
+        <v>1E-3</v>
       </c>
       <c r="C4" s="90" t="s">
         <v>79</v>
@@ -4520,8 +4469,8 @@
       <c r="D4" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="E4" s="260"/>
-      <c r="F4" s="231"/>
+      <c r="E4" s="256"/>
+      <c r="F4" s="225"/>
       <c r="G4" s="69"/>
       <c r="H4" s="69"/>
       <c r="I4" s="69"/>
@@ -4540,8 +4489,8 @@
       <c r="D5" s="129" t="s">
         <v>20</v>
       </c>
-      <c r="E5" s="260"/>
-      <c r="F5" s="232"/>
+      <c r="E5" s="256"/>
+      <c r="F5" s="226"/>
       <c r="G5" s="69"/>
       <c r="H5" s="69"/>
       <c r="I5" s="69"/>
@@ -4552,7 +4501,7 @@
         <v>285</v>
       </c>
       <c r="B6" s="121">
-        <v>7.0000000000000007E-2</v>
+        <v>3.6110000000000003E-2</v>
       </c>
       <c r="C6" s="90" t="s">
         <v>79</v>
@@ -4560,44 +4509,44 @@
       <c r="D6" s="129" t="s">
         <v>81</v>
       </c>
-      <c r="E6" s="260"/>
-      <c r="F6" s="233"/>
+      <c r="E6" s="256"/>
+      <c r="F6" s="227"/>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="126" t="s">
-        <v>286</v>
+      <c r="A7" s="77" t="s">
+        <v>77</v>
       </c>
       <c r="B7" s="121">
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="C7" s="90" t="s">
+        <v>1E-3</v>
+      </c>
+      <c r="C7" s="128" t="s">
         <v>79</v>
       </c>
-      <c r="D7" s="196" t="s">
-        <v>20</v>
-      </c>
-      <c r="E7" s="260"/>
-      <c r="F7" s="233"/>
+      <c r="D7" s="191" t="s">
+        <v>81</v>
+      </c>
+      <c r="E7" s="256"/>
+      <c r="F7" s="227"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
       <c r="B8" s="121">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="C8" s="128" t="s">
+      <c r="C8" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="197" t="s">
+      <c r="D8" s="190" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="260"/>
-      <c r="F8" s="233"/>
+      <c r="E8" s="256"/>
+      <c r="F8" s="227"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B9" s="121">
         <v>9.9999999999999995E-21</v>
@@ -4605,56 +4554,56 @@
       <c r="C9" s="128" t="s">
         <v>79</v>
       </c>
-      <c r="D9" s="197" t="s">
+      <c r="D9" s="191" t="s">
         <v>20</v>
       </c>
-      <c r="F9" s="233"/>
-    </row>
-    <row r="10" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="89" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="121">
+      <c r="E9" s="256"/>
+      <c r="F9" s="227"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="105" t="s">
+        <v>288</v>
+      </c>
+      <c r="B10" s="235">
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="C10" s="128" t="s">
+      <c r="C10" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="D10" s="197" t="s">
-        <v>81</v>
-      </c>
-      <c r="F10" s="233"/>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A11" s="69"/>
-      <c r="B11" s="69"/>
-      <c r="C11" s="69"/>
-      <c r="D11" s="69"/>
-      <c r="E11" s="69"/>
-      <c r="F11" s="69"/>
-      <c r="G11" s="69"/>
-      <c r="H11" s="69"/>
-      <c r="I11" s="69"/>
-      <c r="J11" s="70"/>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" s="69"/>
+      <c r="D10" s="236" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A12" s="69"/>
+      <c r="B12" s="69"/>
+      <c r="C12" s="69"/>
+      <c r="D12" s="69"/>
+      <c r="E12" s="69"/>
+      <c r="F12" s="69"/>
+      <c r="G12" s="69"/>
+      <c r="H12" s="69"/>
+      <c r="I12" s="69"/>
+      <c r="J12" s="70"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A14" s="69"/>
       <c r="B14" s="69"/>
-      <c r="C14" s="69"/>
-      <c r="D14" s="69"/>
-      <c r="E14" s="69"/>
-      <c r="F14" s="69"/>
-      <c r="G14" s="69"/>
-      <c r="H14" s="70"/>
-      <c r="I14" s="69"/>
-      <c r="J14" s="69"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A15" s="69"/>
+      <c r="B15" s="69"/>
+      <c r="C15" s="69"/>
+      <c r="D15" s="69"/>
+      <c r="E15" s="69"/>
+      <c r="F15" s="69"/>
+      <c r="G15" s="69"/>
+      <c r="H15" s="70"/>
+      <c r="I15" s="69"/>
+      <c r="J15" s="69"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E1:E8"/>
+    <mergeCell ref="E1:E9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4663,10 +4612,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:I10"/>
+  <dimension ref="A1:I11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -4690,10 +4639,10 @@
       <c r="C1" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="260" t="s">
+      <c r="D1" s="256" t="s">
         <v>208</v>
       </c>
-      <c r="E1" s="231"/>
+      <c r="E1" s="225"/>
       <c r="F1" s="69"/>
       <c r="G1" s="69"/>
     </row>
@@ -4708,8 +4657,8 @@
       <c r="C2" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="D2" s="260"/>
-      <c r="E2" s="231"/>
+      <c r="D2" s="256"/>
+      <c r="E2" s="225"/>
       <c r="F2" s="69"/>
       <c r="G2" s="69"/>
     </row>
@@ -4724,8 +4673,8 @@
       <c r="C3" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="260"/>
-      <c r="E3" s="231"/>
+      <c r="D3" s="256"/>
+      <c r="E3" s="225"/>
       <c r="F3" s="69"/>
       <c r="G3" s="69"/>
     </row>
@@ -4734,13 +4683,13 @@
         <v>76</v>
       </c>
       <c r="B4" s="121">
-        <v>0.01</v>
+        <v>1E-3</v>
       </c>
       <c r="C4" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="D4" s="260"/>
-      <c r="E4" s="231"/>
+      <c r="D4" s="256"/>
+      <c r="E4" s="225"/>
       <c r="F4" s="69"/>
       <c r="G4" s="69"/>
     </row>
@@ -4755,8 +4704,8 @@
       <c r="C5" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="D5" s="260"/>
-      <c r="E5" s="231"/>
+      <c r="D5" s="256"/>
+      <c r="E5" s="225"/>
       <c r="F5" s="69"/>
       <c r="G5" s="69"/>
     </row>
@@ -4766,51 +4715,52 @@
       </c>
       <c r="B6" s="121">
         <f>Influent!B6</f>
-        <v>7.0000000000000007E-2</v>
+        <v>3.6110000000000003E-2</v>
       </c>
       <c r="C6" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="D6" s="260"/>
-      <c r="E6" s="231"/>
+      <c r="D6" s="256"/>
+      <c r="E6" s="225"/>
       <c r="F6" s="72"/>
       <c r="G6" s="130"/>
       <c r="H6" s="131"/>
       <c r="I6" s="72"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="126" t="s">
+    <row r="7" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A7" s="89" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="133">
+        <v>1E-3</v>
+      </c>
+      <c r="C7" s="134" t="s">
+        <v>79</v>
+      </c>
+      <c r="D7" s="256"/>
+      <c r="E7" s="225"/>
+      <c r="F7" s="72"/>
+      <c r="G7" s="130"/>
+      <c r="H7" s="131"/>
+      <c r="I7" s="72"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A8" s="126" t="s">
         <v>286</v>
-      </c>
-      <c r="B7" s="133">
-        <f>Influent!B7</f>
-        <v>9.9999999999999995E-21</v>
-      </c>
-      <c r="C7" s="119" t="s">
-        <v>79</v>
-      </c>
-      <c r="D7" s="260"/>
-      <c r="E7" s="233"/>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="77" t="s">
-        <v>287</v>
       </c>
       <c r="B8" s="133">
         <f>Influent!B8</f>
         <v>9.9999999999999995E-21</v>
       </c>
-      <c r="C8" s="134" t="s">
+      <c r="C8" s="119" t="s">
         <v>79</v>
       </c>
-      <c r="D8" s="260"/>
-      <c r="E8" s="231"/>
-      <c r="F8" s="69"/>
-      <c r="G8" s="94"/>
+      <c r="D8" s="256"/>
+      <c r="E8" s="227"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
       <c r="B9" s="133">
         <f>Influent!B9</f>
@@ -4819,23 +4769,30 @@
       <c r="C9" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="E9" s="233"/>
-    </row>
-    <row r="10" spans="1:9" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="89" t="s">
-        <v>77</v>
+      <c r="D9" s="256"/>
+      <c r="E9" s="225"/>
+      <c r="F9" s="69"/>
+      <c r="G9" s="94"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A10" s="77" t="s">
+        <v>288</v>
       </c>
       <c r="B10" s="133">
-        <v>0.01</v>
+        <f>Influent!B10</f>
+        <v>9.9999999999999995E-21</v>
       </c>
       <c r="C10" s="134" t="s">
         <v>79</v>
       </c>
-      <c r="E10" s="233"/>
+      <c r="E10" s="227"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="E11" s="227"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="D1:D8"/>
+    <mergeCell ref="D1:D9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4844,10 +4801,10 @@
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I30"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H19" sqref="H19"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4902,12 +4859,12 @@
         <v>83</v>
       </c>
       <c r="G2" s="146">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H2" s="142" t="s">
         <v>80</v>
       </c>
-      <c r="I2" s="260" t="s">
+      <c r="I2" s="256" t="s">
         <v>226</v>
       </c>
     </row>
@@ -4931,12 +4888,12 @@
         <v>83</v>
       </c>
       <c r="G3" s="147">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="H3" s="143" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="260"/>
+      <c r="I3" s="256"/>
     </row>
     <row r="4" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
@@ -4963,7 +4920,7 @@
       <c r="H4" s="143" t="s">
         <v>80</v>
       </c>
-      <c r="I4" s="260"/>
+      <c r="I4" s="256"/>
     </row>
     <row r="5" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
@@ -4990,7 +4947,7 @@
       <c r="H5" s="143" t="s">
         <v>80</v>
       </c>
-      <c r="I5" s="260"/>
+      <c r="I5" s="256"/>
     </row>
     <row r="6" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
@@ -5017,7 +4974,7 @@
       <c r="H6" s="143" t="s">
         <v>80</v>
       </c>
-      <c r="I6" s="260"/>
+      <c r="I6" s="256"/>
     </row>
     <row r="7" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="s">
@@ -5044,17 +5001,17 @@
       <c r="H7" s="143" t="s">
         <v>80</v>
       </c>
-      <c r="I7" s="260"/>
+      <c r="I7" s="256"/>
     </row>
     <row r="8" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="126" t="s">
-        <v>286</v>
-      </c>
-      <c r="B8" s="151" t="s">
+      <c r="A8" s="132" t="s">
+        <v>77</v>
+      </c>
+      <c r="B8" s="149" t="s">
         <v>83</v>
       </c>
       <c r="C8" s="149">
-        <v>-50.75</v>
+        <v>0</v>
       </c>
       <c r="D8" s="149" t="s">
         <v>83</v>
@@ -5065,26 +5022,26 @@
       <c r="F8" s="149" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="192">
+      <c r="G8" s="151">
         <v>2</v>
       </c>
-      <c r="H8" s="143" t="s">
-        <v>300</v>
-      </c>
-      <c r="I8" s="260"/>
-    </row>
-    <row r="9" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A9" s="77" t="s">
-        <v>287</v>
-      </c>
-      <c r="B9" s="151" t="s">
+      <c r="H8" s="93" t="s">
+        <v>80</v>
+      </c>
+      <c r="I8" s="256"/>
+    </row>
+    <row r="9" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A9" s="152" t="s">
+        <v>78</v>
+      </c>
+      <c r="B9" s="149" t="s">
         <v>83</v>
       </c>
       <c r="C9" s="149">
-        <v>-394.35899999999998</v>
-      </c>
-      <c r="D9" s="149" t="s">
-        <v>83</v>
+        <v>-237.18</v>
+      </c>
+      <c r="D9" s="149">
+        <v>-157.30000000000001</v>
       </c>
       <c r="E9" s="149" t="s">
         <v>83</v>
@@ -5095,16 +5052,16 @@
       <c r="G9" s="146">
         <v>2</v>
       </c>
-      <c r="H9" s="143" t="s">
-        <v>300</v>
-      </c>
-      <c r="I9" s="260"/>
-    </row>
-    <row r="10" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A10" s="77" t="s">
-        <v>288</v>
-      </c>
-      <c r="B10" s="151" t="s">
+      <c r="H9" s="73" t="s">
+        <v>80</v>
+      </c>
+      <c r="I9" s="256"/>
+    </row>
+    <row r="10" spans="1:9" s="71" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A10" s="138" t="s">
+        <v>18</v>
+      </c>
+      <c r="B10" s="149" t="s">
         <v>83</v>
       </c>
       <c r="C10" s="149">
@@ -5119,413 +5076,391 @@
       <c r="F10" s="149" t="s">
         <v>83</v>
       </c>
-      <c r="G10" s="192">
+      <c r="G10" s="148">
         <v>2</v>
       </c>
-      <c r="H10" s="143" t="s">
-        <v>300</v>
-      </c>
-      <c r="I10" s="260"/>
-    </row>
-    <row r="11" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A11" s="132" t="s">
-        <v>77</v>
-      </c>
-      <c r="B11" s="149" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" s="149">
-        <v>0</v>
-      </c>
-      <c r="D11" s="149" t="s">
-        <v>83</v>
-      </c>
-      <c r="E11" s="149" t="s">
-        <v>83</v>
-      </c>
-      <c r="F11" s="149" t="s">
-        <v>83</v>
-      </c>
-      <c r="G11" s="152">
-        <v>2</v>
-      </c>
-      <c r="H11" s="93" t="s">
+      <c r="H10" s="74" t="s">
         <v>80</v>
       </c>
-      <c r="I11" s="260"/>
+      <c r="I10" s="256"/>
+    </row>
+    <row r="11" spans="1:9" s="71" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="139" t="s">
+        <v>82</v>
+      </c>
+      <c r="B11" s="144" t="s">
+        <v>216</v>
+      </c>
+      <c r="C11" s="144" t="s">
+        <v>217</v>
+      </c>
+      <c r="D11" s="145" t="s">
+        <v>218</v>
+      </c>
+      <c r="E11" s="144" t="s">
+        <v>219</v>
+      </c>
+      <c r="H11" s="72"/>
     </row>
     <row r="12" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A12" s="153" t="s">
-        <v>78</v>
-      </c>
-      <c r="B12" s="149" t="s">
-        <v>83</v>
-      </c>
-      <c r="C12" s="149">
-        <v>-237.18</v>
-      </c>
-      <c r="D12" s="149">
-        <v>-157.30000000000001</v>
-      </c>
-      <c r="E12" s="149" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="149" t="s">
-        <v>83</v>
-      </c>
-      <c r="G12" s="146">
-        <v>2</v>
-      </c>
-      <c r="H12" s="73" t="s">
-        <v>80</v>
-      </c>
-      <c r="I12" s="260"/>
-    </row>
-    <row r="13" spans="1:9" s="71" customFormat="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="138" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13" s="149" t="s">
-        <v>83</v>
-      </c>
-      <c r="C13" s="149">
-        <v>0</v>
-      </c>
-      <c r="D13" s="149" t="s">
-        <v>83</v>
-      </c>
-      <c r="E13" s="149" t="s">
-        <v>83</v>
-      </c>
-      <c r="F13" s="149" t="s">
-        <v>83</v>
-      </c>
-      <c r="G13" s="148">
-        <v>2</v>
-      </c>
-      <c r="H13" s="74" t="s">
-        <v>80</v>
-      </c>
+      <c r="A12" s="76" t="s">
+        <v>281</v>
+      </c>
+      <c r="B12" s="100">
+        <f>IF(COUNT(B2,C2)=2, EXP(($C$9+B2-C2)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C12" s="100">
+        <v>1.5099999999999999E-5</v>
+      </c>
+      <c r="D12" s="100">
+        <f>IF(COUNT(D2,E2)=2, EXP((E2-D2)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E12" s="100">
+        <f>IF(COUNT(E2,F2)=2, EXP((F2-E2)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="H12" s="72"/>
+      <c r="I12" s="260" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A13" s="77" t="s">
+        <v>282</v>
+      </c>
+      <c r="B13" s="100">
+        <f>IF(COUNT(B3,C3)=2, EXP(($C$9+B3-C3)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C13" s="100">
+        <f>IF(COUNT(C3,D3)=2, EXP((D3-C3)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>2.5092389473500048E-5</v>
+      </c>
+      <c r="D13" s="100">
+        <f>IF(COUNT(D3,E3)=2, EXP((E3-D3)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E13" s="100">
+        <f>IF(COUNT(E3,F3)=2, EXP((F3-E3)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="H13" s="72"/>
       <c r="I13" s="260"/>
     </row>
-    <row r="14" spans="1:9" s="71" customFormat="1" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="139" t="s">
-        <v>82</v>
-      </c>
-      <c r="B14" s="144" t="s">
-        <v>216</v>
-      </c>
-      <c r="C14" s="144" t="s">
-        <v>217</v>
-      </c>
-      <c r="D14" s="145" t="s">
-        <v>218</v>
-      </c>
-      <c r="E14" s="144" t="s">
-        <v>219</v>
+    <row r="14" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A14" s="77" t="s">
+        <v>283</v>
+      </c>
+      <c r="B14" s="100">
+        <f>IF(COUNT(B4,C4)=2, EXP(($C$9+B4-C4)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C14" s="100">
+        <f>IF(COUNT(C4,D4)=2, EXP((D4-C4)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D14" s="100">
+        <f>IF(COUNT(D4,E4)=2, EXP((E4-D4)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E14" s="100">
+        <f>IF(COUNT(E4,F4)=2, EXP((F4-E4)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
       </c>
       <c r="H14" s="72"/>
+      <c r="I14" s="260"/>
     </row>
     <row r="15" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A15" s="76" t="s">
-        <v>281</v>
+      <c r="A15" s="77" t="s">
+        <v>76</v>
       </c>
       <c r="B15" s="100">
-        <f>IF(COUNT(B2,C2)=2, EXP(($C$12+B2-C2)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <f>IF(COUNT(B5,C5)=2, EXP(($C$9+B5-C5)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="C15" s="100">
-        <v>1.5099999999999999E-5</v>
+        <f>IF(COUNT(C5,D5)=2, EXP((D5-C5)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>7.0008373922189771E-7</v>
       </c>
       <c r="D15" s="100">
-        <f>IF(COUNT(D2,E2)=2, EXP((E2-D2)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
+        <f>IF(COUNT(D5,E5)=2, EXP((E5-D5)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>9.7842822173758576E-11</v>
       </c>
       <c r="E15" s="100">
-        <f>IF(COUNT(E2,F2)=2, EXP((F2-E2)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <f>IF(COUNT(E5,F5)=2, EXP((F5-E5)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="H15" s="72"/>
-      <c r="I15" s="264" t="s">
-        <v>227</v>
-      </c>
+      <c r="I15" s="260"/>
     </row>
     <row r="16" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A16" s="77" t="s">
-        <v>282</v>
+        <v>284</v>
       </c>
       <c r="B16" s="100">
-        <f>IF(COUNT(B3,C3)=2, EXP(($C$12+B3-C3)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <f>IF(COUNT(B6,C6)=2, EXP(($C$9+B6-C6)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="C16" s="100">
-        <f>IF(COUNT(C3,D3)=2, EXP((D3-C3)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>2.5092389473500048E-5</v>
+        <f>IF(COUNT(C6,D6)=2, EXP((D6-C6)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
       </c>
       <c r="D16" s="100">
-        <f>IF(COUNT(D3,E3)=2, EXP((E3-D3)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <f>IF(COUNT(D6,E6)=2, EXP((E6-D6)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="E16" s="100">
-        <f>IF(COUNT(E3,F3)=2, EXP((F3-E3)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <f>IF(COUNT(E6,F6)=2, EXP((F6-E6)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="H16" s="72"/>
-      <c r="I16" s="264"/>
-    </row>
-    <row r="17" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="I16" s="260"/>
+    </row>
+    <row r="17" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A17" s="77" t="s">
-        <v>283</v>
+        <v>285</v>
       </c>
       <c r="B17" s="100">
-        <f>IF(COUNT(B4,C4)=2, EXP(($C$12+B4-C4)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <f>IF(COUNT(B7,C7)=2, EXP(($C$9+B7-C7)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="C17" s="100">
-        <f>IF(COUNT(C4,D4)=2, EXP((D4-C4)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D17" s="100">
-        <f>IF(COUNT(D4,E4)=2, EXP((E4-D4)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E17" s="100">
-        <f>IF(COUNT(E4,F4)=2, EXP((F4-E4)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H17" s="72"/>
-      <c r="I17" s="264"/>
-    </row>
-    <row r="18" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A18" s="77" t="s">
-        <v>76</v>
-      </c>
-      <c r="B18" s="100">
-        <f>IF(COUNT(B5,C5)=2, EXP(($C$12+B5-C5)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C18" s="100">
-        <f>IF(COUNT(C5,D5)=2, EXP((D5-C5)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>7.0008373922189771E-7</v>
-      </c>
-      <c r="D18" s="100">
-        <f>IF(COUNT(D5,E5)=2, EXP((E5-D5)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>9.7842822173758576E-11</v>
-      </c>
-      <c r="E18" s="100">
-        <f>IF(COUNT(E5,F5)=2, EXP((F5-E5)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H18" s="72"/>
-      <c r="I18" s="264"/>
-    </row>
-    <row r="19" spans="1:9" s="71" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A19" s="77" t="s">
-        <v>284</v>
-      </c>
-      <c r="B19" s="100">
-        <f>IF(COUNT(B6,C6)=2, EXP(($C$12+B6-C6)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C19" s="100">
-        <f>IF(COUNT(C6,D6)=2, EXP((D6-C6)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D19" s="100">
-        <f>IF(COUNT(D6,E6)=2, EXP((E6-D6)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E19" s="100">
-        <f>IF(COUNT(E6,F6)=2, EXP((F6-E6)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="H19" s="72"/>
-      <c r="I19" s="264"/>
-    </row>
-    <row r="20" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A20" s="77" t="s">
-        <v>285</v>
-      </c>
-      <c r="B20" s="100">
-        <f>IF(COUNT(B7,C7)=2, EXP(($C$12+B7-C7)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C20" s="100">
         <f>IF(COUNT(C7,D7)=2, EXP((D7-C7)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
         <v>1.1219060033069472E-9</v>
       </c>
+      <c r="D17" s="100">
+        <f>IF(COUNT(D7,E7)=2, EXP((E7-D7)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E17" s="100">
+        <f>IF(COUNT(E7,F7)=2, EXP((F7-E7)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F17" s="71"/>
+      <c r="I17" s="260"/>
+    </row>
+    <row r="18" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A18" s="132" t="s">
+        <v>77</v>
+      </c>
+      <c r="B18" s="100">
+        <f>IF(COUNT(B8,C8)=2, EXP(($C$9+B8-C8)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C18" s="100">
+        <f>IF(COUNT(C8,D8)=2, EXP((D8-C8)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="D18" s="100">
+        <f>IF(COUNT(D8,E8)=2, EXP((E8-D8)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E18" s="100">
+        <f>IF(COUNT(E8,F8)=2, EXP((F8-E8)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F18" s="71"/>
+      <c r="I18" s="260"/>
+    </row>
+    <row r="19" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A19" s="152" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="100">
+        <f>IF(COUNT(B9,C9)=2, EXP(($C$9+B9-C9)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C19" s="100">
+        <f>IF(COUNT(C9,D9)=2, EXP((D9-C9)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>2.8818342317080507E-14</v>
+      </c>
+      <c r="D19" s="100">
+        <f>IF(COUNT(D9,E9)=2, EXP((E9-D9)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="E19" s="100">
+        <f>IF(COUNT(E9,F9)=2, EXP((F9-E9)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="F19" s="71"/>
+      <c r="H19" s="71"/>
+      <c r="I19" s="260"/>
+    </row>
+    <row r="20" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="138" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="100">
+        <f>IF(COUNT(B10,C10)=2, EXP(($C$9+B10-C10)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
+      <c r="C20" s="100">
+        <f>IF(COUNT(C10,D10)=2, EXP((D10-C10)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <v>0</v>
+      </c>
       <c r="D20" s="100">
-        <f>IF(COUNT(D7,E7)=2, EXP((E7-D7)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <f>IF(COUNT(D10,E10)=2, EXP((E10-D10)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="E20" s="100">
-        <f>IF(COUNT(E7,F7)=2, EXP((F7-E7)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
+        <f>IF(COUNT(E10,F10)=2, EXP((F10-E10)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
         <v>0</v>
       </c>
       <c r="F20" s="71"/>
-      <c r="I20" s="264"/>
-    </row>
-    <row r="21" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A21" s="126" t="s">
-        <v>286</v>
-      </c>
-      <c r="B21" s="100">
-        <f>IF(COUNT(B8,C8)=2, EXP(($C$12+B8-C8)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C21" s="100">
-        <f>IF(COUNT(C8,D8)=2, EXP((D8-C8)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D21" s="100">
-        <f>IF(COUNT(D8,E8)=2, EXP((E8-D8)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E21" s="100">
-        <f>IF(COUNT(E8,F8)=2, EXP((F8-E8)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F21" s="71"/>
-      <c r="I21" s="264"/>
+      <c r="I20" s="260"/>
+    </row>
+    <row r="21" spans="1:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="257" t="s">
+        <v>215</v>
+      </c>
+      <c r="B21" s="258"/>
+      <c r="C21" s="258"/>
+      <c r="D21" s="258"/>
+      <c r="E21" s="258"/>
+      <c r="F21" s="259"/>
     </row>
     <row r="22" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A22" s="77" t="s">
-        <v>287</v>
-      </c>
-      <c r="B22" s="100">
-        <f>IF(COUNT(B9,C9)=2, EXP(($C$12+B9-C9)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C22" s="100">
-        <f>IF(COUNT(C9,D9)=2, EXP((D9-C9)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D22" s="100">
-        <f>IF(COUNT(D9,E9)=2, EXP((E9-D9)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E22" s="100">
-        <f>IF(COUNT(E9,F9)=2, EXP((F9-E9)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F22" s="71"/>
-      <c r="I22" s="264"/>
+      <c r="A22" s="76" t="s">
+        <v>281</v>
+      </c>
+      <c r="B22" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="C22" s="150">
+        <v>0</v>
+      </c>
+      <c r="D22" s="150">
+        <v>-1</v>
+      </c>
+      <c r="E22" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="F22" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="I22" s="260" t="s">
+        <v>228</v>
+      </c>
     </row>
     <row r="23" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
       <c r="A23" s="77" t="s">
-        <v>288</v>
-      </c>
-      <c r="B23" s="100">
-        <f>IF(COUNT(B10,C10)=2, EXP(($C$12+B10-C10)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C23" s="100">
-        <f>IF(COUNT(C10,D10)=2, EXP((D10-C10)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D23" s="100">
-        <f>IF(COUNT(D10,E10)=2, EXP((E10-D10)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E23" s="100">
-        <f>IF(COUNT(E10,F10)=2, EXP((F10-E10)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F23" s="71"/>
-      <c r="I23" s="264"/>
+        <v>282</v>
+      </c>
+      <c r="B23" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" s="150">
+        <v>0</v>
+      </c>
+      <c r="D23" s="150">
+        <v>-1</v>
+      </c>
+      <c r="E23" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="I23" s="260"/>
     </row>
     <row r="24" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A24" s="132" t="s">
+      <c r="A24" s="77" t="s">
+        <v>283</v>
+      </c>
+      <c r="B24" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="C24" s="150">
+        <v>0</v>
+      </c>
+      <c r="D24" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="E24" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="F24" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="I24" s="260"/>
+    </row>
+    <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A25" s="77" t="s">
+        <v>76</v>
+      </c>
+      <c r="B25" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="C25" s="150">
+        <v>0</v>
+      </c>
+      <c r="D25" s="150">
+        <v>-1</v>
+      </c>
+      <c r="E25" s="150">
+        <v>-2</v>
+      </c>
+      <c r="F25" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="I25" s="260"/>
+    </row>
+    <row r="26" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A26" s="77" t="s">
+        <v>284</v>
+      </c>
+      <c r="B26" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="C26" s="150">
+        <v>0</v>
+      </c>
+      <c r="D26" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="E26" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="F26" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="I26" s="260"/>
+    </row>
+    <row r="27" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A27" s="77" t="s">
+        <v>285</v>
+      </c>
+      <c r="B27" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="C27" s="150">
+        <v>1</v>
+      </c>
+      <c r="D27" s="150">
+        <v>0</v>
+      </c>
+      <c r="E27" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="F27" s="150" t="s">
+        <v>84</v>
+      </c>
+      <c r="I27" s="260"/>
+    </row>
+    <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A28" s="132" t="s">
         <v>77</v>
-      </c>
-      <c r="B24" s="100">
-        <f>IF(COUNT(B11,C11)=2, EXP(($C$12+B11-C11)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C24" s="100">
-        <f>IF(COUNT(C11,D11)=2, EXP((D11-C11)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D24" s="100">
-        <f>IF(COUNT(D11,E11)=2, EXP((E11-D11)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E24" s="100">
-        <f>IF(COUNT(E11,F11)=2, EXP((F11-E11)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F24" s="71"/>
-      <c r="I24" s="264"/>
-    </row>
-    <row r="25" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A25" s="153" t="s">
-        <v>78</v>
-      </c>
-      <c r="B25" s="100">
-        <f>IF(COUNT(B12,C12)=2, EXP(($C$12+B12-C12)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C25" s="100">
-        <f>IF(COUNT(C12,D12)=2, EXP((D12-C12)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>2.8818342317080507E-14</v>
-      </c>
-      <c r="D25" s="100">
-        <f>IF(COUNT(D12,E12)=2, EXP((E12-D12)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E25" s="100">
-        <f>IF(COUNT(E12,F12)=2, EXP((F12-E12)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F25" s="71"/>
-      <c r="H25" s="71"/>
-      <c r="I25" s="264"/>
-    </row>
-    <row r="26" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="138" t="s">
-        <v>18</v>
-      </c>
-      <c r="B26" s="100">
-        <f>IF(COUNT(B13,C13)=2, EXP(($C$12+B13-C13)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="C26" s="100">
-        <f>IF(COUNT(C13,D13)=2, EXP((D13-C13)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="D26" s="100">
-        <f>IF(COUNT(D13,E13)=2, EXP((E13-D13)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="E26" s="100">
-        <f>IF(COUNT(E13,F13)=2, EXP((F13-E13)/-(Parameters!$B$12*Parameters!$B$6)), 0)</f>
-        <v>0</v>
-      </c>
-      <c r="F26" s="71"/>
-      <c r="I26" s="264"/>
-    </row>
-    <row r="27" spans="1:9" ht="28.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="261" t="s">
-        <v>215</v>
-      </c>
-      <c r="B27" s="262"/>
-      <c r="C27" s="262"/>
-      <c r="D27" s="262"/>
-      <c r="E27" s="262"/>
-      <c r="F27" s="263"/>
-    </row>
-    <row r="28" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A28" s="76" t="s">
-        <v>281</v>
       </c>
       <c r="B28" s="150" t="s">
         <v>84</v>
       </c>
       <c r="C28" s="150">
-        <v>0</v>
-      </c>
-      <c r="D28" s="150">
-        <v>-1</v>
+        <v>1</v>
+      </c>
+      <c r="D28" s="150" t="s">
+        <v>84</v>
       </c>
       <c r="E28" s="150" t="s">
         <v>84</v>
@@ -5533,13 +5468,11 @@
       <c r="F28" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="I28" s="264" t="s">
-        <v>228</v>
-      </c>
+      <c r="I28" s="260"/>
     </row>
     <row r="29" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A29" s="77" t="s">
-        <v>282</v>
+      <c r="A29" s="152" t="s">
+        <v>78</v>
       </c>
       <c r="B29" s="150" t="s">
         <v>84</v>
@@ -5556,17 +5489,17 @@
       <c r="F29" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="I29" s="264"/>
-    </row>
-    <row r="30" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A30" s="77" t="s">
-        <v>283</v>
+      <c r="I29" s="260"/>
+    </row>
+    <row r="30" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="138" t="s">
+        <v>18</v>
       </c>
       <c r="B30" s="150" t="s">
         <v>84</v>
       </c>
       <c r="C30" s="150">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D30" s="150" t="s">
         <v>84</v>
@@ -5577,210 +5510,21 @@
       <c r="F30" s="150" t="s">
         <v>84</v>
       </c>
-      <c r="I30" s="264"/>
-    </row>
-    <row r="31" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A31" s="77" t="s">
-        <v>76</v>
-      </c>
-      <c r="B31" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="C31" s="150">
-        <v>0</v>
-      </c>
-      <c r="D31" s="150">
-        <v>-1</v>
-      </c>
-      <c r="E31" s="150">
-        <v>-2</v>
-      </c>
-      <c r="F31" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="I31" s="264"/>
-    </row>
-    <row r="32" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A32" s="77" t="s">
-        <v>284</v>
-      </c>
-      <c r="B32" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="C32" s="150">
-        <v>0</v>
-      </c>
-      <c r="D32" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="E32" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="F32" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="I32" s="264"/>
-    </row>
-    <row r="33" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A33" s="77" t="s">
-        <v>285</v>
-      </c>
-      <c r="B33" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="C33" s="150">
-        <v>1</v>
-      </c>
-      <c r="D33" s="150">
-        <v>0</v>
-      </c>
-      <c r="E33" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="F33" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="I33" s="264"/>
-    </row>
-    <row r="34" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A34" s="126" t="s">
-        <v>286</v>
-      </c>
-      <c r="B34" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="C34" s="150">
-        <v>0</v>
-      </c>
-      <c r="D34" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="E34" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="F34" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="I34" s="264"/>
-    </row>
-    <row r="35" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A35" s="77" t="s">
-        <v>287</v>
-      </c>
-      <c r="B35" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="C35" s="150">
-        <v>0</v>
-      </c>
-      <c r="D35" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="E35" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="F35" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="I35" s="264"/>
-    </row>
-    <row r="36" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A36" s="77" t="s">
-        <v>288</v>
-      </c>
-      <c r="B36" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="C36" s="150">
-        <v>0</v>
-      </c>
-      <c r="D36" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="E36" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="F36" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="I36" s="264"/>
-    </row>
-    <row r="37" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A37" s="132" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="C37" s="150">
-        <v>1</v>
-      </c>
-      <c r="D37" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="E37" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="F37" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="I37" s="264"/>
-    </row>
-    <row r="38" spans="1:9" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A38" s="153" t="s">
-        <v>78</v>
-      </c>
-      <c r="B38" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="C38" s="150">
-        <v>0</v>
-      </c>
-      <c r="D38" s="150">
-        <v>-1</v>
-      </c>
-      <c r="E38" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="F38" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="I38" s="264"/>
-    </row>
-    <row r="39" spans="1:9" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="138" t="s">
-        <v>18</v>
-      </c>
-      <c r="B39" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="C39" s="150">
-        <v>1</v>
-      </c>
-      <c r="D39" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="E39" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="F39" s="150" t="s">
-        <v>84</v>
-      </c>
-      <c r="I39" s="264"/>
+      <c r="I30" s="260"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="A27:F27"/>
-    <mergeCell ref="I2:I13"/>
-    <mergeCell ref="I15:I26"/>
-    <mergeCell ref="I28:I39"/>
+    <mergeCell ref="A21:F21"/>
+    <mergeCell ref="I2:I10"/>
+    <mergeCell ref="I12:I20"/>
+    <mergeCell ref="I22:I30"/>
   </mergeCells>
-  <conditionalFormatting sqref="B15:E26">
+  <conditionalFormatting sqref="B12:E20">
     <cfRule type="cellIs" dxfId="8" priority="7" operator="equal">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:F13 B15:E26 B28:F39">
+  <conditionalFormatting sqref="B2:F10 B12:E20 B22:F30">
     <cfRule type="containsText" dxfId="7" priority="60" operator="containsText" text="NA">
       <formula>NOT(ISERROR(SEARCH("NA",B2)))</formula>
     </cfRule>
@@ -5799,7 +5543,7 @@
   <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5827,7 +5571,7 @@
       <c r="F1" s="135" t="s">
         <v>285</v>
       </c>
-      <c r="G1" s="265" t="s">
+      <c r="G1" s="261" t="s">
         <v>268</v>
       </c>
     </row>
@@ -5850,7 +5594,7 @@
       <c r="F2" s="100">
         <v>1E-4</v>
       </c>
-      <c r="G2" s="265"/>
+      <c r="G2" s="261"/>
     </row>
     <row r="3" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
@@ -5871,7 +5615,7 @@
       <c r="F3" s="100">
         <v>1E-4</v>
       </c>
-      <c r="G3" s="265"/>
+      <c r="G3" s="261"/>
     </row>
     <row r="4" spans="1:7" ht="13.95" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
@@ -5892,13 +5636,13 @@
       <c r="F4" s="100">
         <v>1E-4</v>
       </c>
-      <c r="G4" s="265"/>
+      <c r="G4" s="261"/>
     </row>
     <row r="5" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G5" s="169"/>
+      <c r="G5" s="168"/>
     </row>
     <row r="6" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="G6" s="169"/>
+      <c r="G6" s="168"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -5919,7 +5663,7 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5946,7 +5690,7 @@
       <c r="F1" s="135" t="s">
         <v>285</v>
       </c>
-      <c r="G1" s="265" t="s">
+      <c r="G1" s="261" t="s">
         <v>267</v>
       </c>
     </row>
@@ -5969,7 +5713,7 @@
       <c r="F2" s="100">
         <v>0</v>
       </c>
-      <c r="G2" s="265"/>
+      <c r="G2" s="261"/>
     </row>
     <row r="3" spans="1:7" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
@@ -5990,7 +5734,7 @@
       <c r="F3" s="100">
         <v>1.8E-3</v>
       </c>
-      <c r="G3" s="265"/>
+      <c r="G3" s="261"/>
     </row>
     <row r="4" spans="1:7" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
@@ -6011,7 +5755,7 @@
       <c r="F4" s="100">
         <v>0</v>
       </c>
-      <c r="G4" s="265"/>
+      <c r="G4" s="261"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6028,10 +5772,10 @@
 
 <file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1EB714E2-DC7C-4045-B67C-ABD3059A2B98}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6047,153 +5791,161 @@
       <c r="A1" s="77" t="s">
         <v>281</v>
       </c>
-      <c r="B1" s="240">
+      <c r="B1" s="234">
         <v>0</v>
       </c>
       <c r="C1" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="D1" s="236">
-        <v>0</v>
-      </c>
-      <c r="E1" s="257" t="s">
-        <v>301</v>
+      <c r="D1" s="230">
+        <v>0</v>
+      </c>
+      <c r="E1" s="253" t="s">
+        <v>300</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="77" t="s">
         <v>282</v>
       </c>
-      <c r="B2" s="238">
+      <c r="B2" s="232">
         <v>0</v>
       </c>
       <c r="C2" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="D2" s="236">
-        <v>0</v>
-      </c>
-      <c r="E2" s="258"/>
+      <c r="D2" s="230">
+        <v>0</v>
+      </c>
+      <c r="E2" s="254"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
         <v>283</v>
       </c>
-      <c r="B3" s="238">
-        <v>1.4E-3</v>
+      <c r="B3" s="232">
+        <f>0.001161687</f>
+        <v>1.161687E-3</v>
       </c>
       <c r="C3" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="D3" s="236">
+      <c r="D3" s="230">
         <v>-1</v>
       </c>
-      <c r="E3" s="258"/>
+      <c r="E3" s="254"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="238">
-        <v>3.5000000000000003E-2</v>
+      <c r="B4" s="232">
+        <f>0.02713983</f>
+        <v>2.713983E-2</v>
       </c>
       <c r="C4" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="D4" s="236">
+      <c r="D4" s="230">
         <v>-1</v>
       </c>
-      <c r="E4" s="258"/>
+      <c r="E4" s="254"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="s">
         <v>284</v>
       </c>
-      <c r="B5" s="238">
-        <v>7.7999999999999999E-4</v>
+      <c r="B5" s="232">
+        <v>7.3842500000000002E-4</v>
       </c>
       <c r="C5" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="D5" s="236">
+      <c r="D5" s="230">
         <v>-1</v>
       </c>
-      <c r="E5" s="258"/>
+      <c r="E5" s="254"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="s">
         <v>285</v>
       </c>
-      <c r="B6" s="238">
+      <c r="B6" s="232">
         <v>0</v>
       </c>
       <c r="C6" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="D6" s="236">
-        <v>0</v>
-      </c>
-      <c r="E6" s="258"/>
+      <c r="D6" s="230">
+        <v>0</v>
+      </c>
+      <c r="E6" s="254"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="126" t="s">
-        <v>286</v>
-      </c>
-      <c r="B7" s="238">
-        <v>1.4E-3</v>
+      <c r="A7" s="77" t="s">
+        <v>77</v>
+      </c>
+      <c r="B7" s="232">
+        <v>0</v>
       </c>
       <c r="C7" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="D7" s="236">
-        <v>1</v>
-      </c>
-      <c r="E7" s="258"/>
+      <c r="D7" s="230">
+        <v>0</v>
+      </c>
+      <c r="E7" s="254"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
-        <v>287</v>
-      </c>
-      <c r="B8" s="238">
-        <v>3.5000000000000003E-2</v>
+        <v>286</v>
+      </c>
+      <c r="B8" s="232">
+        <f>0.001161687</f>
+        <v>1.161687E-3</v>
       </c>
       <c r="C8" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="D8" s="236">
+      <c r="D8" s="230">
         <v>1</v>
       </c>
-      <c r="E8" s="258"/>
+      <c r="E8" s="254"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="s">
-        <v>288</v>
-      </c>
-      <c r="B9" s="238">
-        <v>7.7999999999999999E-4</v>
+        <v>287</v>
+      </c>
+      <c r="B9" s="232">
+        <f>0.02713983</f>
+        <v>2.713983E-2</v>
       </c>
       <c r="C9" s="90" t="s">
         <v>294</v>
       </c>
-      <c r="D9" s="236">
+      <c r="D9" s="230">
         <v>1</v>
       </c>
-      <c r="E9" s="258"/>
+      <c r="E9" s="254"/>
     </row>
     <row r="10" spans="1:5" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="89" t="s">
-        <v>77</v>
-      </c>
-      <c r="B10" s="239">
-        <v>0</v>
+        <v>288</v>
+      </c>
+      <c r="B10" s="233">
+        <v>7.3842500000000002E-4</v>
       </c>
       <c r="C10" s="92" t="s">
         <v>294</v>
       </c>
-      <c r="D10" s="237">
-        <v>0</v>
-      </c>
-      <c r="E10" s="259"/>
+      <c r="D10" s="231">
+        <v>1</v>
+      </c>
+      <c r="E10" s="254"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="B11" s="69"/>
+      <c r="D11" s="63"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6247,8 +5999,8 @@
       <c r="E1" s="135" t="s">
         <v>224</v>
       </c>
-      <c r="F1" s="260" t="s">
-        <v>302</v>
+      <c r="F1" s="256" t="s">
+        <v>301</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
@@ -6267,7 +6019,7 @@
       <c r="E2" s="137" t="s">
         <v>84</v>
       </c>
-      <c r="F2" s="260"/>
+      <c r="F2" s="256"/>
     </row>
     <row r="3" spans="1:6" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="s">
@@ -6285,7 +6037,7 @@
       <c r="E3" s="137" t="s">
         <v>84</v>
       </c>
-      <c r="F3" s="260"/>
+      <c r="F3" s="256"/>
     </row>
     <row r="4" spans="1:6" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="89" t="s">
@@ -6303,7 +6055,7 @@
       <c r="E4" s="137" t="s">
         <v>84</v>
       </c>
-      <c r="F4" s="260"/>
+      <c r="F4" s="256"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -6315,13 +6067,13 @@
 
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
-  <dimension ref="A1:J14"/>
+  <dimension ref="A1:J11"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I16" sqref="I16"/>
+      <selection pane="bottomRight" activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -6337,49 +6089,49 @@
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1" s="69"/>
-      <c r="B1" s="266" t="s">
+      <c r="B1" s="262" t="s">
         <v>291</v>
       </c>
-      <c r="C1" s="267"/>
-      <c r="D1" s="268"/>
-      <c r="E1" s="266" t="s">
+      <c r="C1" s="263"/>
+      <c r="D1" s="264"/>
+      <c r="E1" s="262" t="s">
         <v>289</v>
       </c>
-      <c r="F1" s="267"/>
-      <c r="G1" s="268"/>
-      <c r="H1" s="267" t="s">
+      <c r="F1" s="263"/>
+      <c r="G1" s="264"/>
+      <c r="H1" s="263" t="s">
         <v>290</v>
       </c>
-      <c r="I1" s="267"/>
-      <c r="J1" s="268"/>
+      <c r="I1" s="263"/>
+      <c r="J1" s="264"/>
     </row>
     <row r="2" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="234"/>
-      <c r="B2" s="154" t="s">
+      <c r="A2" s="228"/>
+      <c r="B2" s="153" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="155" t="s">
+      <c r="C2" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="156" t="s">
+      <c r="D2" s="155" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="154" t="s">
+      <c r="E2" s="153" t="s">
         <v>73</v>
       </c>
-      <c r="F2" s="155" t="s">
+      <c r="F2" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="G2" s="156" t="s">
+      <c r="G2" s="155" t="s">
         <v>75</v>
       </c>
-      <c r="H2" s="155" t="s">
+      <c r="H2" s="154" t="s">
         <v>73</v>
       </c>
-      <c r="I2" s="155" t="s">
+      <c r="I2" s="154" t="s">
         <v>74</v>
       </c>
-      <c r="J2" s="156" t="s">
+      <c r="J2" s="155" t="s">
         <v>75</v>
       </c>
     </row>
@@ -6396,22 +6148,22 @@
       <c r="D3" s="102">
         <v>0</v>
       </c>
-      <c r="E3" s="160">
+      <c r="E3" s="159">
         <v>0</v>
       </c>
       <c r="F3" s="102">
         <v>0</v>
       </c>
-      <c r="G3" s="161">
-        <v>0</v>
-      </c>
-      <c r="H3" s="160">
+      <c r="G3" s="160">
+        <v>0</v>
+      </c>
+      <c r="H3" s="159">
         <v>0</v>
       </c>
       <c r="I3" s="102">
         <v>0</v>
       </c>
-      <c r="J3" s="161">
+      <c r="J3" s="160">
         <v>0</v>
       </c>
     </row>
@@ -6419,31 +6171,31 @@
       <c r="A4" s="77" t="s">
         <v>282</v>
       </c>
-      <c r="B4" s="162">
+      <c r="B4" s="161">
         <v>2</v>
       </c>
       <c r="C4" s="136">
         <v>0</v>
       </c>
-      <c r="D4" s="163">
-        <v>0</v>
-      </c>
-      <c r="E4" s="162">
+      <c r="D4" s="162">
+        <v>0</v>
+      </c>
+      <c r="E4" s="161">
         <v>-1</v>
       </c>
       <c r="F4" s="136">
         <v>-0.5</v>
       </c>
-      <c r="G4" s="163">
-        <v>0</v>
-      </c>
-      <c r="H4" s="162">
+      <c r="G4" s="162">
+        <v>0</v>
+      </c>
+      <c r="H4" s="161">
         <v>0</v>
       </c>
       <c r="I4" s="136">
         <v>0</v>
       </c>
-      <c r="J4" s="163">
+      <c r="J4" s="162">
         <v>0</v>
       </c>
     </row>
@@ -6451,31 +6203,31 @@
       <c r="A5" s="77" t="s">
         <v>283</v>
       </c>
-      <c r="B5" s="162">
+      <c r="B5" s="161">
         <v>0</v>
       </c>
       <c r="C5" s="136">
         <v>0</v>
       </c>
-      <c r="D5" s="163">
-        <v>0</v>
-      </c>
-      <c r="E5" s="162">
+      <c r="D5" s="162">
+        <v>0</v>
+      </c>
+      <c r="E5" s="161">
         <v>1</v>
       </c>
       <c r="F5" s="136">
         <v>0</v>
       </c>
-      <c r="G5" s="163">
-        <v>0</v>
-      </c>
-      <c r="H5" s="162">
+      <c r="G5" s="162">
+        <v>0</v>
+      </c>
+      <c r="H5" s="161">
         <v>0.25</v>
       </c>
       <c r="I5" s="136">
         <v>0</v>
       </c>
-      <c r="J5" s="163">
+      <c r="J5" s="162">
         <v>0</v>
       </c>
     </row>
@@ -6483,31 +6235,31 @@
       <c r="A6" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B6" s="162">
+      <c r="B6" s="161">
         <v>0</v>
       </c>
       <c r="C6" s="136">
         <v>0</v>
       </c>
-      <c r="D6" s="163">
-        <v>0</v>
-      </c>
-      <c r="E6" s="162">
+      <c r="D6" s="162">
+        <v>0</v>
+      </c>
+      <c r="E6" s="161">
         <v>1</v>
       </c>
       <c r="F6" s="136">
         <v>0</v>
       </c>
-      <c r="G6" s="163">
-        <v>0</v>
-      </c>
-      <c r="H6" s="162">
+      <c r="G6" s="162">
+        <v>0</v>
+      </c>
+      <c r="H6" s="161">
         <v>-0.25</v>
       </c>
       <c r="I6" s="136">
         <v>-1</v>
       </c>
-      <c r="J6" s="163">
+      <c r="J6" s="162">
         <v>0</v>
       </c>
     </row>
@@ -6515,31 +6267,31 @@
       <c r="A7" s="77" t="s">
         <v>284</v>
       </c>
-      <c r="B7" s="164">
+      <c r="B7" s="163">
         <v>2</v>
       </c>
       <c r="C7" s="136">
         <v>0.5</v>
       </c>
-      <c r="D7" s="165">
-        <v>0</v>
-      </c>
-      <c r="E7" s="164">
+      <c r="D7" s="164">
+        <v>0</v>
+      </c>
+      <c r="E7" s="163">
         <v>0</v>
       </c>
       <c r="F7" s="136">
         <v>0</v>
       </c>
-      <c r="G7" s="165">
-        <v>0</v>
-      </c>
-      <c r="H7" s="164">
+      <c r="G7" s="164">
+        <v>0</v>
+      </c>
+      <c r="H7" s="163">
         <v>-1</v>
       </c>
       <c r="I7" s="136">
         <v>-2</v>
       </c>
-      <c r="J7" s="165">
+      <c r="J7" s="164">
         <v>0</v>
       </c>
     </row>
@@ -6547,223 +6299,127 @@
       <c r="A8" s="77" t="s">
         <v>285</v>
       </c>
-      <c r="B8" s="164">
-        <v>0</v>
-      </c>
-      <c r="C8" s="157">
+      <c r="B8" s="163">
+        <v>0</v>
+      </c>
+      <c r="C8" s="156">
         <v>-0.2</v>
       </c>
-      <c r="D8" s="165">
-        <v>0</v>
-      </c>
-      <c r="E8" s="164">
-        <v>0</v>
-      </c>
-      <c r="F8" s="157">
+      <c r="D8" s="164">
+        <v>0</v>
+      </c>
+      <c r="E8" s="163">
+        <v>0</v>
+      </c>
+      <c r="F8" s="156">
         <v>-0.2</v>
       </c>
-      <c r="G8" s="165">
-        <v>0</v>
-      </c>
-      <c r="H8" s="164">
-        <v>0</v>
-      </c>
-      <c r="I8" s="157">
+      <c r="G8" s="164">
+        <v>0</v>
+      </c>
+      <c r="H8" s="163">
+        <v>0</v>
+      </c>
+      <c r="I8" s="156">
         <v>-0.2</v>
       </c>
-      <c r="J8" s="165">
+      <c r="J8" s="164">
         <v>0</v>
       </c>
     </row>
     <row r="9" spans="1:10" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="126" t="s">
-        <v>286</v>
-      </c>
-      <c r="B9" s="189">
-        <v>0</v>
-      </c>
-      <c r="C9" s="190">
-        <v>0</v>
-      </c>
-      <c r="D9" s="191">
-        <v>0</v>
-      </c>
-      <c r="E9" s="189">
-        <v>0</v>
-      </c>
-      <c r="F9" s="190">
-        <v>0</v>
-      </c>
-      <c r="G9" s="191">
-        <v>0</v>
-      </c>
-      <c r="H9" s="189">
-        <v>0</v>
-      </c>
-      <c r="I9" s="190">
-        <v>0</v>
-      </c>
-      <c r="J9" s="191">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="77" t="s">
-        <v>287</v>
-      </c>
-      <c r="B10" s="162">
-        <v>0</v>
-      </c>
-      <c r="C10" s="136">
-        <v>0</v>
-      </c>
-      <c r="D10" s="163">
-        <v>0</v>
-      </c>
-      <c r="E10" s="162">
-        <v>0</v>
-      </c>
-      <c r="F10" s="136">
-        <v>0</v>
-      </c>
-      <c r="G10" s="163">
-        <v>0</v>
-      </c>
-      <c r="H10" s="162">
-        <v>0</v>
-      </c>
-      <c r="I10" s="136">
-        <v>0</v>
-      </c>
-      <c r="J10" s="163">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="77" t="s">
-        <v>288</v>
-      </c>
-      <c r="B11" s="186">
-        <v>0</v>
-      </c>
-      <c r="C11" s="187">
-        <v>0</v>
-      </c>
-      <c r="D11" s="188">
-        <v>0</v>
-      </c>
-      <c r="E11" s="186">
-        <v>0</v>
-      </c>
-      <c r="F11" s="187">
-        <v>0</v>
-      </c>
-      <c r="G11" s="188">
-        <v>0</v>
-      </c>
-      <c r="H11" s="186">
-        <v>0</v>
-      </c>
-      <c r="I11" s="187">
-        <v>0</v>
-      </c>
-      <c r="J11" s="188">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" s="63" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="132" t="s">
+      <c r="A9" s="132" t="s">
         <v>77</v>
       </c>
-      <c r="B12" s="158">
-        <v>0</v>
-      </c>
-      <c r="C12" s="159">
-        <v>0</v>
-      </c>
-      <c r="D12" s="166">
-        <v>0</v>
-      </c>
-      <c r="E12" s="158">
-        <v>0</v>
-      </c>
-      <c r="F12" s="159">
-        <v>0</v>
-      </c>
-      <c r="G12" s="166">
-        <v>0</v>
-      </c>
-      <c r="H12" s="158">
-        <v>0</v>
-      </c>
-      <c r="I12" s="159">
-        <v>0</v>
-      </c>
-      <c r="J12" s="166">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A13" s="153" t="s">
+      <c r="B9" s="157">
+        <v>0</v>
+      </c>
+      <c r="C9" s="158">
+        <v>0</v>
+      </c>
+      <c r="D9" s="165">
+        <v>0</v>
+      </c>
+      <c r="E9" s="157">
+        <v>0</v>
+      </c>
+      <c r="F9" s="158">
+        <v>0</v>
+      </c>
+      <c r="G9" s="165">
+        <v>0</v>
+      </c>
+      <c r="H9" s="157">
+        <v>0</v>
+      </c>
+      <c r="I9" s="158">
+        <v>0</v>
+      </c>
+      <c r="J9" s="165">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" s="152" t="s">
         <v>78</v>
       </c>
-      <c r="B13" s="189">
+      <c r="B10" s="185">
         <v>-2</v>
       </c>
-      <c r="C13" s="190">
+      <c r="C10" s="186">
         <v>0.1</v>
       </c>
-      <c r="D13" s="191">
-        <v>0</v>
-      </c>
-      <c r="E13" s="189">
+      <c r="D10" s="187">
+        <v>0</v>
+      </c>
+      <c r="E10" s="185">
         <v>-1</v>
       </c>
-      <c r="F13" s="190">
+      <c r="F10" s="186">
         <v>0.6</v>
       </c>
-      <c r="G13" s="191">
-        <v>0</v>
-      </c>
-      <c r="H13" s="189">
+      <c r="G10" s="187">
+        <v>0</v>
+      </c>
+      <c r="H10" s="185">
         <v>0.75</v>
       </c>
-      <c r="I13" s="190">
+      <c r="I10" s="186">
         <v>2.6</v>
       </c>
-      <c r="J13" s="191">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A14" s="138" t="s">
+      <c r="J10" s="187">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="138" t="s">
         <v>18</v>
       </c>
-      <c r="B14" s="97">
+      <c r="B11" s="97">
         <v>1</v>
       </c>
-      <c r="C14" s="167">
+      <c r="C11" s="166">
         <v>-0.05</v>
       </c>
-      <c r="D14" s="168">
-        <v>0</v>
-      </c>
-      <c r="E14" s="97">
-        <v>0</v>
-      </c>
-      <c r="F14" s="167">
+      <c r="D11" s="167">
+        <v>0</v>
+      </c>
+      <c r="E11" s="97">
+        <v>0</v>
+      </c>
+      <c r="F11" s="166">
         <v>-0.3</v>
       </c>
-      <c r="G14" s="168">
-        <v>0</v>
-      </c>
-      <c r="H14" s="97">
+      <c r="G11" s="167">
+        <v>0</v>
+      </c>
+      <c r="H11" s="97">
         <v>-0.25</v>
       </c>
-      <c r="I14" s="167">
+      <c r="I11" s="166">
         <v>-0.8</v>
       </c>
-      <c r="J14" s="168">
+      <c r="J11" s="167">
         <v>0</v>
       </c>
     </row>
@@ -6773,7 +6429,7 @@
     <mergeCell ref="E1:G1"/>
     <mergeCell ref="H1:J1"/>
   </mergeCells>
-  <conditionalFormatting sqref="B3:J14">
+  <conditionalFormatting sqref="B3:J11">
     <cfRule type="cellIs" dxfId="0" priority="3" operator="equal">
       <formula>0</formula>
     </cfRule>
@@ -6829,30 +6485,30 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:40" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="S2" s="241" t="s">
-        <v>0</v>
-      </c>
-      <c r="T2" s="241"/>
-      <c r="U2" s="241"/>
-      <c r="V2" s="241"/>
-      <c r="W2" s="241" t="s">
+      <c r="S2" s="237" t="s">
+        <v>0</v>
+      </c>
+      <c r="T2" s="237"/>
+      <c r="U2" s="237"/>
+      <c r="V2" s="237"/>
+      <c r="W2" s="237" t="s">
         <v>1</v>
       </c>
-      <c r="X2" s="241"/>
-      <c r="Y2" s="241"/>
-      <c r="Z2" s="241"/>
-      <c r="AA2" s="241" t="s">
+      <c r="X2" s="237"/>
+      <c r="Y2" s="237"/>
+      <c r="Z2" s="237"/>
+      <c r="AA2" s="237" t="s">
         <v>2</v>
       </c>
-      <c r="AB2" s="241"/>
-      <c r="AC2" s="241"/>
-      <c r="AD2" s="241"/>
-      <c r="AE2" s="241" t="s">
+      <c r="AB2" s="237"/>
+      <c r="AC2" s="237"/>
+      <c r="AD2" s="237"/>
+      <c r="AE2" s="237" t="s">
         <v>3</v>
       </c>
-      <c r="AF2" s="241"/>
-      <c r="AG2" s="241"/>
-      <c r="AH2" s="241"/>
+      <c r="AF2" s="237"/>
+      <c r="AG2" s="237"/>
+      <c r="AH2" s="237"/>
       <c r="AK2" s="3" t="s">
         <v>4</v>
       </c>
@@ -8305,10 +7961,10 @@
         <f>1/F17</f>
         <v>3.4893748785390075E-2</v>
       </c>
-      <c r="J17" s="242" t="s">
+      <c r="J17" s="238" t="s">
         <v>54</v>
       </c>
-      <c r="K17" s="245" t="s">
+      <c r="K17" s="241" t="s">
         <v>55</v>
       </c>
       <c r="R17" s="43" t="s">
@@ -8408,8 +8064,8 @@
         <f t="shared" ref="G18:G19" si="9">1/F18</f>
         <v>2.1521507799447302E-2</v>
       </c>
-      <c r="J18" s="243"/>
-      <c r="K18" s="246"/>
+      <c r="J18" s="239"/>
+      <c r="K18" s="242"/>
       <c r="R18" s="46" t="s">
         <v>57</v>
       </c>
@@ -8507,8 +8163,8 @@
         <f t="shared" si="9"/>
         <v>5.6574173051404053E-2</v>
       </c>
-      <c r="J19" s="243"/>
-      <c r="K19" s="246"/>
+      <c r="J19" s="239"/>
+      <c r="K19" s="242"/>
       <c r="R19" s="46" t="s">
         <v>59</v>
       </c>
@@ -8588,8 +8244,8 @@
       <c r="D20" s="19"/>
       <c r="E20" s="19"/>
       <c r="F20" s="36"/>
-      <c r="J20" s="243"/>
-      <c r="K20" s="246"/>
+      <c r="J20" s="239"/>
+      <c r="K20" s="242"/>
       <c r="R20" s="46" t="s">
         <v>60</v>
       </c>
@@ -8670,8 +8326,8 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="59"/>
-      <c r="J21" s="243"/>
-      <c r="K21" s="246"/>
+      <c r="J21" s="239"/>
+      <c r="K21" s="242"/>
       <c r="R21" s="46" t="s">
         <v>61</v>
       </c>
@@ -8752,8 +8408,8 @@
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="59"/>
-      <c r="J22" s="243"/>
-      <c r="K22" s="246"/>
+      <c r="J22" s="239"/>
+      <c r="K22" s="242"/>
       <c r="R22" s="46" t="s">
         <v>62</v>
       </c>
@@ -8834,8 +8490,8 @@
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="59"/>
-      <c r="J23" s="243"/>
-      <c r="K23" s="246"/>
+      <c r="J23" s="239"/>
+      <c r="K23" s="242"/>
       <c r="R23" s="48" t="s">
         <v>23</v>
       </c>
@@ -8916,8 +8572,8 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="59"/>
-      <c r="J24" s="243"/>
-      <c r="K24" s="246"/>
+      <c r="J24" s="239"/>
+      <c r="K24" s="242"/>
       <c r="V24" s="51" t="s">
         <v>63</v>
       </c>
@@ -8938,8 +8594,8 @@
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="59"/>
-      <c r="J25" s="243"/>
-      <c r="K25" s="246"/>
+      <c r="J25" s="239"/>
+      <c r="K25" s="242"/>
     </row>
     <row r="26" spans="2:36" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B26" s="58"/>
@@ -8948,14 +8604,14 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="59"/>
-      <c r="J26" s="243"/>
-      <c r="K26" s="246"/>
-      <c r="N26" s="248" t="s">
+      <c r="J26" s="239"/>
+      <c r="K26" s="242"/>
+      <c r="N26" s="244" t="s">
         <v>64</v>
       </c>
-      <c r="O26" s="249"/>
-      <c r="P26" s="249"/>
-      <c r="Q26" s="250"/>
+      <c r="O26" s="245"/>
+      <c r="P26" s="245"/>
+      <c r="Q26" s="246"/>
       <c r="R26" s="52" t="s">
         <v>65</v>
       </c>
@@ -9031,14 +8687,14 @@
       <c r="E27" s="19"/>
       <c r="F27" s="19"/>
       <c r="G27" s="59"/>
-      <c r="J27" s="243"/>
-      <c r="K27" s="246"/>
-      <c r="N27" s="248" t="s">
+      <c r="J27" s="239"/>
+      <c r="K27" s="242"/>
+      <c r="N27" s="244" t="s">
         <v>66</v>
       </c>
-      <c r="O27" s="249"/>
-      <c r="P27" s="249"/>
-      <c r="Q27" s="250"/>
+      <c r="O27" s="245"/>
+      <c r="P27" s="245"/>
+      <c r="Q27" s="246"/>
       <c r="R27" s="55" t="s">
         <v>67</v>
       </c>
@@ -9114,8 +8770,8 @@
       <c r="E28" s="19"/>
       <c r="F28" s="19"/>
       <c r="G28" s="59"/>
-      <c r="J28" s="243"/>
-      <c r="K28" s="246"/>
+      <c r="J28" s="239"/>
+      <c r="K28" s="242"/>
       <c r="O28" s="27"/>
       <c r="P28" s="27"/>
       <c r="Q28" s="27"/>
@@ -9127,24 +8783,24 @@
       <c r="E29" s="19"/>
       <c r="F29" s="19"/>
       <c r="G29" s="59"/>
-      <c r="J29" s="243"/>
-      <c r="K29" s="246"/>
+      <c r="J29" s="239"/>
+      <c r="K29" s="242"/>
     </row>
     <row r="30" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="J30" s="243"/>
-      <c r="K30" s="246"/>
+      <c r="J30" s="239"/>
+      <c r="K30" s="242"/>
     </row>
     <row r="31" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="J31" s="243"/>
-      <c r="K31" s="246"/>
+      <c r="J31" s="239"/>
+      <c r="K31" s="242"/>
     </row>
     <row r="32" spans="2:36" x14ac:dyDescent="0.3">
-      <c r="J32" s="243"/>
-      <c r="K32" s="246"/>
+      <c r="J32" s="239"/>
+      <c r="K32" s="242"/>
     </row>
     <row r="33" spans="10:26" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J33" s="244"/>
-      <c r="K33" s="247"/>
+      <c r="J33" s="240"/>
+      <c r="K33" s="243"/>
     </row>
     <row r="34" spans="10:26" x14ac:dyDescent="0.3">
       <c r="U34" s="82"/>
@@ -9293,7 +8949,7 @@
   <dimension ref="B2:AL36"/>
   <sheetViews>
     <sheetView topLeftCell="G1" zoomScale="70" zoomScaleNormal="70" zoomScalePageLayoutView="125" workbookViewId="0">
-      <selection activeCell="S23" sqref="S23"/>
+      <selection activeCell="M19" sqref="M19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9326,27 +8982,27 @@
   <sheetData>
     <row r="2" spans="7:38" ht="21.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="G2" s="1"/>
-      <c r="S2" s="241" t="s">
+      <c r="S2" s="237" t="s">
         <v>291</v>
       </c>
-      <c r="T2" s="241"/>
-      <c r="U2" s="241"/>
-      <c r="V2" s="241"/>
-      <c r="W2" s="241"/>
-      <c r="X2" s="241" t="s">
+      <c r="T2" s="237"/>
+      <c r="U2" s="237"/>
+      <c r="V2" s="237"/>
+      <c r="W2" s="237"/>
+      <c r="X2" s="237" t="s">
         <v>289</v>
       </c>
-      <c r="Y2" s="241"/>
-      <c r="Z2" s="241"/>
-      <c r="AA2" s="241"/>
-      <c r="AB2" s="241"/>
-      <c r="AC2" s="241" t="s">
+      <c r="Y2" s="237"/>
+      <c r="Z2" s="237"/>
+      <c r="AA2" s="237"/>
+      <c r="AB2" s="237"/>
+      <c r="AC2" s="237" t="s">
         <v>290</v>
       </c>
-      <c r="AD2" s="241"/>
-      <c r="AE2" s="241"/>
-      <c r="AF2" s="241"/>
-      <c r="AG2" s="241"/>
+      <c r="AD2" s="237"/>
+      <c r="AE2" s="237"/>
+      <c r="AF2" s="237"/>
+      <c r="AG2" s="237"/>
       <c r="AI2" s="3" t="s">
         <v>4</v>
       </c>
@@ -10322,33 +9978,33 @@
       <c r="S13" s="40">
         <v>0</v>
       </c>
-      <c r="T13" s="235">
-        <v>0</v>
-      </c>
-      <c r="U13" s="235">
+      <c r="T13" s="229">
+        <v>0</v>
+      </c>
+      <c r="U13" s="229">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="V13" s="235">
+      <c r="V13" s="229">
         <v>1</v>
       </c>
-      <c r="W13" s="235">
+      <c r="W13" s="229">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
       <c r="X13" s="40">
         <v>0</v>
       </c>
-      <c r="Y13" s="235">
-        <v>0</v>
-      </c>
-      <c r="Z13" s="235">
-        <v>0</v>
-      </c>
-      <c r="AA13" s="235">
+      <c r="Y13" s="229">
+        <v>0</v>
+      </c>
+      <c r="Z13" s="229">
+        <v>0</v>
+      </c>
+      <c r="AA13" s="229">
         <v>1</v>
       </c>
-      <c r="AB13" s="235">
+      <c r="AB13" s="229">
         <f t="shared" si="3"/>
         <v>1</v>
       </c>
@@ -10362,7 +10018,7 @@
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="AF13" s="235">
+      <c r="AF13" s="229">
         <v>1</v>
       </c>
       <c r="AG13" s="28">
@@ -10373,10 +10029,10 @@
     </row>
     <row r="14" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G14" s="1"/>
-      <c r="J14" s="242" t="s">
+      <c r="J14" s="238" t="s">
         <v>54</v>
       </c>
-      <c r="K14" s="245" t="s">
+      <c r="K14" s="241" t="s">
         <v>55</v>
       </c>
       <c r="R14" s="43" t="s">
@@ -10446,8 +10102,8 @@
     </row>
     <row r="15" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G15" s="1"/>
-      <c r="J15" s="243"/>
-      <c r="K15" s="246"/>
+      <c r="J15" s="239"/>
+      <c r="K15" s="242"/>
       <c r="R15" s="46" t="s">
         <v>57</v>
       </c>
@@ -10515,8 +10171,8 @@
     </row>
     <row r="16" spans="7:38" x14ac:dyDescent="0.3">
       <c r="G16" s="1"/>
-      <c r="J16" s="243"/>
-      <c r="K16" s="246"/>
+      <c r="J16" s="239"/>
+      <c r="K16" s="242"/>
       <c r="R16" s="46" t="s">
         <v>59</v>
       </c>
@@ -10584,8 +10240,8 @@
     </row>
     <row r="17" spans="2:34" x14ac:dyDescent="0.3">
       <c r="G17" s="1"/>
-      <c r="J17" s="243"/>
-      <c r="K17" s="246"/>
+      <c r="J17" s="239"/>
+      <c r="K17" s="242"/>
       <c r="R17" s="46" t="s">
         <v>60</v>
       </c>
@@ -10653,8 +10309,8 @@
     </row>
     <row r="18" spans="2:34" x14ac:dyDescent="0.3">
       <c r="G18" s="1"/>
-      <c r="J18" s="243"/>
-      <c r="K18" s="246"/>
+      <c r="J18" s="239"/>
+      <c r="K18" s="242"/>
       <c r="R18" s="46" t="s">
         <v>61</v>
       </c>
@@ -10722,8 +10378,8 @@
     </row>
     <row r="19" spans="2:34" x14ac:dyDescent="0.3">
       <c r="G19" s="1"/>
-      <c r="J19" s="243"/>
-      <c r="K19" s="246"/>
+      <c r="J19" s="239"/>
+      <c r="K19" s="242"/>
       <c r="R19" s="46" t="s">
         <v>62</v>
       </c>
@@ -10796,8 +10452,8 @@
       <c r="E20" s="19"/>
       <c r="F20" s="19"/>
       <c r="G20" s="59"/>
-      <c r="J20" s="243"/>
-      <c r="K20" s="246"/>
+      <c r="J20" s="239"/>
+      <c r="K20" s="242"/>
       <c r="R20" s="48" t="s">
         <v>23</v>
       </c>
@@ -10870,8 +10526,8 @@
       <c r="E21" s="19"/>
       <c r="F21" s="19"/>
       <c r="G21" s="59"/>
-      <c r="J21" s="243"/>
-      <c r="K21" s="246"/>
+      <c r="J21" s="239"/>
+      <c r="K21" s="242"/>
     </row>
     <row r="22" spans="2:34" ht="15.6" x14ac:dyDescent="0.3">
       <c r="B22" s="58"/>
@@ -10880,8 +10536,8 @@
       <c r="E22" s="19"/>
       <c r="F22" s="19"/>
       <c r="G22" s="59"/>
-      <c r="J22" s="243"/>
-      <c r="K22" s="246"/>
+      <c r="J22" s="239"/>
+      <c r="K22" s="242"/>
     </row>
     <row r="23" spans="2:34" ht="17.399999999999999" x14ac:dyDescent="0.3">
       <c r="B23" s="58"/>
@@ -10890,14 +10546,14 @@
       <c r="E23" s="19"/>
       <c r="F23" s="19"/>
       <c r="G23" s="59"/>
-      <c r="J23" s="243"/>
-      <c r="K23" s="246"/>
-      <c r="N23" s="248" t="s">
+      <c r="J23" s="239"/>
+      <c r="K23" s="242"/>
+      <c r="N23" s="244" t="s">
         <v>64</v>
       </c>
-      <c r="O23" s="249"/>
-      <c r="P23" s="249"/>
-      <c r="Q23" s="250"/>
+      <c r="O23" s="245"/>
+      <c r="P23" s="245"/>
+      <c r="Q23" s="246"/>
       <c r="R23" s="52" t="s">
         <v>65</v>
       </c>
@@ -10969,14 +10625,14 @@
       <c r="E24" s="19"/>
       <c r="F24" s="19"/>
       <c r="G24" s="59"/>
-      <c r="J24" s="243"/>
-      <c r="K24" s="246"/>
-      <c r="N24" s="248" t="s">
+      <c r="J24" s="239"/>
+      <c r="K24" s="242"/>
+      <c r="N24" s="244" t="s">
         <v>66</v>
       </c>
-      <c r="O24" s="249"/>
-      <c r="P24" s="249"/>
-      <c r="Q24" s="250"/>
+      <c r="O24" s="245"/>
+      <c r="P24" s="245"/>
+      <c r="Q24" s="246"/>
       <c r="R24" s="55" t="s">
         <v>67</v>
       </c>
@@ -11048,8 +10704,8 @@
       <c r="E25" s="19"/>
       <c r="F25" s="19"/>
       <c r="G25" s="59"/>
-      <c r="J25" s="243"/>
-      <c r="K25" s="246"/>
+      <c r="J25" s="239"/>
+      <c r="K25" s="242"/>
       <c r="O25" s="27"/>
       <c r="P25" s="27"/>
       <c r="Q25" s="27"/>
@@ -11061,24 +10717,24 @@
       <c r="E26" s="19"/>
       <c r="F26" s="19"/>
       <c r="G26" s="59"/>
-      <c r="J26" s="243"/>
-      <c r="K26" s="246"/>
+      <c r="J26" s="239"/>
+      <c r="K26" s="242"/>
     </row>
     <row r="27" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="J27" s="243"/>
-      <c r="K27" s="246"/>
+      <c r="J27" s="239"/>
+      <c r="K27" s="242"/>
     </row>
     <row r="28" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="J28" s="243"/>
-      <c r="K28" s="246"/>
+      <c r="J28" s="239"/>
+      <c r="K28" s="242"/>
     </row>
     <row r="29" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="J29" s="243"/>
-      <c r="K29" s="246"/>
+      <c r="J29" s="239"/>
+      <c r="K29" s="242"/>
     </row>
     <row r="30" spans="2:34" x14ac:dyDescent="0.3">
-      <c r="J30" s="244"/>
-      <c r="K30" s="247"/>
+      <c r="J30" s="240"/>
+      <c r="K30" s="243"/>
     </row>
     <row r="31" spans="2:34" x14ac:dyDescent="0.3">
       <c r="AB31"/>
@@ -11148,11 +10804,11 @@
         <f>Discretization!A16</f>
         <v>Dynamic dT</v>
       </c>
-      <c r="B1" s="223" t="b">
+      <c r="B1" s="217" t="b">
         <f>Discretization!B16</f>
         <v>1</v>
       </c>
-      <c r="C1" s="251" t="s">
+      <c r="C1" s="247" t="s">
         <v>236</v>
       </c>
     </row>
@@ -11161,115 +10817,115 @@
         <f>Parameters!A2</f>
         <v>Variable HRT</v>
       </c>
-      <c r="B2" s="224" t="b">
+      <c r="B2" s="218" t="b">
         <f>Parameters!B2</f>
         <v>0</v>
       </c>
-      <c r="C2" s="252"/>
+      <c r="C2" s="248"/>
     </row>
     <row r="3" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A3" s="77" t="str">
         <f>Bacteria!A6</f>
         <v>Initialisation method</v>
       </c>
-      <c r="B3" s="224" t="str">
+      <c r="B3" s="218" t="str">
         <f>Bacteria!B6</f>
         <v>granule</v>
       </c>
-      <c r="C3" s="252"/>
+      <c r="C3" s="248"/>
     </row>
     <row r="4" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A4" s="77" t="str">
         <f>Bacteria!A12</f>
         <v>kDist</v>
       </c>
-      <c r="B4" s="224">
+      <c r="B4" s="218">
         <f>Bacteria!B12</f>
         <v>1</v>
       </c>
-      <c r="C4" s="252"/>
+      <c r="C4" s="248"/>
     </row>
     <row r="5" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A5" s="77" t="str">
         <f>Bacteria!A13</f>
         <v>Inactivation enabled</v>
       </c>
-      <c r="B5" s="224" t="b">
+      <c r="B5" s="218" t="b">
         <f>Bacteria!B13</f>
         <v>1</v>
       </c>
-      <c r="C5" s="252"/>
+      <c r="C5" s="248"/>
     </row>
     <row r="6" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A6" s="77" t="str">
         <f>Solver!A4</f>
         <v>pH bulk concentration corrected</v>
       </c>
-      <c r="B6" s="224" t="b">
+      <c r="B6" s="218" t="b">
         <f>Solver!B4</f>
-        <v>1</v>
-      </c>
-      <c r="C6" s="252"/>
+        <v>0</v>
+      </c>
+      <c r="C6" s="248"/>
     </row>
     <row r="7" spans="1:3" ht="14.4" x14ac:dyDescent="0.25">
       <c r="A7" s="77" t="str">
         <f>Solver!A2</f>
         <v>pH solving included</v>
       </c>
-      <c r="B7" s="224" t="b">
+      <c r="B7" s="218" t="b">
         <f>Solver!B2</f>
-        <v>1</v>
-      </c>
-      <c r="C7" s="252"/>
+        <v>0</v>
+      </c>
+      <c r="C7" s="248"/>
     </row>
     <row r="8" spans="1:3" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="89" t="str">
         <f>Solver!A5</f>
         <v>Speciation included</v>
       </c>
-      <c r="B8" s="225" t="b">
+      <c r="B8" s="219" t="b">
         <f>Solver!B5</f>
         <v>1</v>
       </c>
-      <c r="C8" s="252"/>
+      <c r="C8" s="248"/>
     </row>
     <row r="9" spans="1:3" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="77" t="str">
         <f>Solver!A11</f>
         <v>Structure model</v>
       </c>
-      <c r="B9" s="224" t="b">
+      <c r="B9" s="218" t="b">
         <f>Solver!B11</f>
         <v>0</v>
       </c>
-      <c r="C9" s="252"/>
+      <c r="C9" s="248"/>
     </row>
     <row r="10" spans="1:3" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="89" t="str">
         <f>Solver!A12</f>
         <v>Structure model type</v>
       </c>
-      <c r="B10" s="225" t="str">
+      <c r="B10" s="219" t="str">
         <f>Solver!B12</f>
         <v>Neut</v>
       </c>
-      <c r="C10" s="253"/>
+      <c r="C10" s="249"/>
     </row>
     <row r="11" spans="1:3" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C11" s="169"/>
+      <c r="C11" s="168"/>
     </row>
     <row r="12" spans="1:3" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C12" s="169"/>
+      <c r="C12" s="168"/>
     </row>
     <row r="13" spans="1:3" ht="13.2" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C13" s="169"/>
+      <c r="C13" s="168"/>
     </row>
     <row r="14" spans="1:3" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="169"/>
+      <c r="C14" s="168"/>
     </row>
     <row r="15" spans="1:3" ht="13.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B15" s="226"/>
-      <c r="C15" s="169"/>
+      <c r="B15" s="220"/>
+      <c r="C15" s="168"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -11283,8 +10939,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0800-000000000000}">
   <dimension ref="A1:G29"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11309,10 +10965,10 @@
       <c r="D1" s="107" t="s">
         <v>110</v>
       </c>
-      <c r="E1" s="254" t="s">
+      <c r="E1" s="250" t="s">
         <v>117</v>
       </c>
-      <c r="F1" s="227"/>
+      <c r="F1" s="221"/>
     </row>
     <row r="2" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
@@ -11327,8 +10983,8 @@
       <c r="D2" s="107" t="s">
         <v>111</v>
       </c>
-      <c r="E2" s="254"/>
-      <c r="F2" s="227"/>
+      <c r="E2" s="250"/>
+      <c r="F2" s="221"/>
     </row>
     <row r="3" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
@@ -11344,7 +11000,7 @@
       <c r="D3" s="107" t="s">
         <v>104</v>
       </c>
-      <c r="E3" s="254"/>
+      <c r="E3" s="250"/>
     </row>
     <row r="4" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
@@ -11360,7 +11016,7 @@
       <c r="D4" s="107" t="s">
         <v>105</v>
       </c>
-      <c r="E4" s="254"/>
+      <c r="E4" s="250"/>
     </row>
     <row r="5" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
@@ -11375,7 +11031,7 @@
       <c r="D5" s="107" t="s">
         <v>106</v>
       </c>
-      <c r="E5" s="254"/>
+      <c r="E5" s="250"/>
     </row>
     <row r="6" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
@@ -11390,7 +11046,7 @@
       <c r="D6" s="107" t="s">
         <v>107</v>
       </c>
-      <c r="E6" s="254"/>
+      <c r="E6" s="250"/>
     </row>
     <row r="7" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A7" s="77" t="s">
@@ -11406,7 +11062,7 @@
       <c r="D7" s="107" t="s">
         <v>108</v>
       </c>
-      <c r="E7" s="254"/>
+      <c r="E7" s="250"/>
     </row>
     <row r="8" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="89" t="s">
@@ -11422,8 +11078,8 @@
       <c r="D8" s="108" t="s">
         <v>109</v>
       </c>
-      <c r="E8" s="255"/>
-      <c r="F8" s="227"/>
+      <c r="E8" s="251"/>
+      <c r="F8" s="221"/>
     </row>
     <row r="9" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="76" t="s">
@@ -11438,10 +11094,10 @@
       <c r="D9" s="109" t="s">
         <v>112</v>
       </c>
-      <c r="E9" s="256" t="s">
+      <c r="E9" s="252" t="s">
         <v>118</v>
       </c>
-      <c r="F9" s="227"/>
+      <c r="F9" s="221"/>
       <c r="G9" s="69"/>
     </row>
     <row r="10" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
@@ -11457,7 +11113,7 @@
       <c r="D10" s="107" t="s">
         <v>128</v>
       </c>
-      <c r="E10" s="254"/>
+      <c r="E10" s="250"/>
     </row>
     <row r="11" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A11" s="77" t="s">
@@ -11473,7 +11129,7 @@
       <c r="D11" s="107" t="s">
         <v>130</v>
       </c>
-      <c r="E11" s="254"/>
+      <c r="E11" s="250"/>
     </row>
     <row r="12" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A12" s="77" t="s">
@@ -11488,7 +11144,7 @@
       <c r="D12" s="107" t="s">
         <v>134</v>
       </c>
-      <c r="E12" s="254"/>
+      <c r="E12" s="250"/>
     </row>
     <row r="13" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A13" s="77" t="s">
@@ -11503,7 +11159,7 @@
       <c r="D13" s="107" t="s">
         <v>115</v>
       </c>
-      <c r="E13" s="254"/>
+      <c r="E13" s="250"/>
     </row>
     <row r="14" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="77" t="s">
@@ -11518,7 +11174,7 @@
       <c r="D14" s="107" t="s">
         <v>270</v>
       </c>
-      <c r="E14" s="254"/>
+      <c r="E14" s="250"/>
     </row>
     <row r="15" spans="1:7" ht="15" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A15" s="89" t="s">
@@ -11534,7 +11190,7 @@
       <c r="D15" s="108" t="s">
         <v>116</v>
       </c>
-      <c r="E15" s="255"/>
+      <c r="E15" s="251"/>
     </row>
     <row r="16" spans="1:7" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A16" s="104" t="s">
@@ -11549,7 +11205,7 @@
       <c r="D16" s="110" t="s">
         <v>138</v>
       </c>
-      <c r="E16" s="256" t="s">
+      <c r="E16" s="252" t="s">
         <v>151</v>
       </c>
     </row>
@@ -11566,7 +11222,7 @@
       <c r="D17" s="107" t="s">
         <v>126</v>
       </c>
-      <c r="E17" s="254"/>
+      <c r="E17" s="250"/>
     </row>
     <row r="18" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A18" s="77" t="s">
@@ -11582,7 +11238,7 @@
       <c r="D18" s="107" t="s">
         <v>127</v>
       </c>
-      <c r="E18" s="254"/>
+      <c r="E18" s="250"/>
     </row>
     <row r="19" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A19" s="77" t="s">
@@ -11597,7 +11253,7 @@
       <c r="D19" s="107" t="s">
         <v>264</v>
       </c>
-      <c r="E19" s="254"/>
+      <c r="E19" s="250"/>
     </row>
     <row r="20" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A20" s="77" t="s">
@@ -11613,7 +11269,7 @@
       <c r="D20" s="107" t="s">
         <v>129</v>
       </c>
-      <c r="E20" s="254"/>
+      <c r="E20" s="250"/>
     </row>
     <row r="21" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A21" s="77" t="s">
@@ -11628,7 +11284,7 @@
       <c r="D21" s="107" t="s">
         <v>135</v>
       </c>
-      <c r="E21" s="254"/>
+      <c r="E21" s="250"/>
     </row>
     <row r="22" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A22" s="105" t="s">
@@ -11643,7 +11299,7 @@
       <c r="D22" s="111" t="s">
         <v>136</v>
       </c>
-      <c r="E22" s="254"/>
+      <c r="E22" s="250"/>
     </row>
     <row r="23" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A23" s="77" t="s">
@@ -11658,7 +11314,7 @@
       <c r="D23" s="112" t="s">
         <v>145</v>
       </c>
-      <c r="E23" s="254"/>
+      <c r="E23" s="250"/>
     </row>
     <row r="24" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A24" s="77" t="s">
@@ -11673,7 +11329,7 @@
       <c r="D24" s="112" t="s">
         <v>146</v>
       </c>
-      <c r="E24" s="254"/>
+      <c r="E24" s="250"/>
     </row>
     <row r="25" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A25" s="77" t="s">
@@ -11688,7 +11344,7 @@
       <c r="D25" s="112" t="s">
         <v>147</v>
       </c>
-      <c r="E25" s="254"/>
+      <c r="E25" s="250"/>
     </row>
     <row r="26" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A26" s="77" t="s">
@@ -11703,13 +11359,13 @@
       <c r="D26" s="112" t="s">
         <v>148</v>
       </c>
-      <c r="E26" s="254"/>
+      <c r="E26" s="250"/>
     </row>
     <row r="27" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A27" s="77" t="s">
         <v>149</v>
       </c>
-      <c r="B27" s="184">
+      <c r="B27" s="183">
         <v>0.2</v>
       </c>
       <c r="C27" s="90" t="s">
@@ -11718,7 +11374,7 @@
       <c r="D27" s="112" t="s">
         <v>263</v>
       </c>
-      <c r="E27" s="254"/>
+      <c r="E27" s="250"/>
     </row>
     <row r="28" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A28" s="77" t="s">
@@ -11733,7 +11389,7 @@
       <c r="D28" s="112" t="s">
         <v>260</v>
       </c>
-      <c r="E28" s="254"/>
+      <c r="E28" s="250"/>
     </row>
     <row r="29" spans="1:5" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A29" s="89" t="s">
@@ -11748,7 +11404,7 @@
       <c r="D29" s="113" t="s">
         <v>150</v>
       </c>
-      <c r="E29" s="255"/>
+      <c r="E29" s="251"/>
     </row>
   </sheetData>
   <mergeCells count="3">
@@ -11776,7 +11432,7 @@
   <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -11792,16 +11448,16 @@
       <c r="A1" s="76" t="s">
         <v>90</v>
       </c>
-      <c r="B1" s="198">
+      <c r="B1" s="192">
         <v>12</v>
       </c>
       <c r="C1" s="91" t="s">
         <v>91</v>
       </c>
-      <c r="D1" s="199" t="s">
+      <c r="D1" s="193" t="s">
         <v>161</v>
       </c>
-      <c r="E1" s="228"/>
+      <c r="E1" s="222"/>
     </row>
     <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="77" t="s">
@@ -11813,7 +11469,7 @@
       <c r="C2" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="194" t="s">
+      <c r="D2" s="188" t="s">
         <v>157</v>
       </c>
       <c r="E2" s="69"/>
@@ -11829,7 +11485,7 @@
       <c r="C3" s="90" t="s">
         <v>79</v>
       </c>
-      <c r="D3" s="194" t="s">
+      <c r="D3" s="188" t="s">
         <v>156</v>
       </c>
       <c r="E3" s="69"/>
@@ -11844,7 +11500,7 @@
       <c r="C4" s="119" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="200" t="s">
+      <c r="D4" s="194" t="s">
         <v>237</v>
       </c>
       <c r="E4" s="69"/>
@@ -11859,7 +11515,7 @@
       <c r="C5" s="90" t="s">
         <v>17</v>
       </c>
-      <c r="D5" s="194" t="s">
+      <c r="D5" s="188" t="s">
         <v>160</v>
       </c>
       <c r="E5" s="69"/>
@@ -11868,14 +11524,14 @@
       <c r="A6" s="77" t="s">
         <v>221</v>
       </c>
-      <c r="B6" s="201">
+      <c r="B6" s="195">
         <f>B5+273.15</f>
         <v>308.14999999999998</v>
       </c>
       <c r="C6" s="90" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="194" t="s">
+      <c r="D6" s="188" t="s">
         <v>220</v>
       </c>
       <c r="E6" s="69"/>
@@ -11884,13 +11540,13 @@
       <c r="A7" s="77" t="s">
         <v>154</v>
       </c>
-      <c r="B7" s="202">
+      <c r="B7" s="196">
         <v>7</v>
       </c>
       <c r="C7" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D7" s="194" t="s">
+      <c r="D7" s="188" t="s">
         <v>162</v>
       </c>
       <c r="E7" s="69"/>
@@ -11899,14 +11555,14 @@
       <c r="A8" s="77" t="s">
         <v>275</v>
       </c>
-      <c r="B8" s="202">
+      <c r="B8" s="196">
         <f>200/24</f>
         <v>8.3333333333333339</v>
       </c>
       <c r="C8" s="90" t="s">
         <v>277</v>
       </c>
-      <c r="D8" s="194" t="s">
+      <c r="D8" s="188" t="s">
         <v>278</v>
       </c>
       <c r="E8" s="69"/>
@@ -11915,13 +11571,13 @@
       <c r="A9" s="77" t="s">
         <v>276</v>
       </c>
-      <c r="B9" s="202">
+      <c r="B9" s="196">
         <v>1.0129999999999999</v>
       </c>
       <c r="C9" s="90" t="s">
         <v>279</v>
       </c>
-      <c r="D9" s="194" t="s">
+      <c r="D9" s="188" t="s">
         <v>280</v>
       </c>
       <c r="E9" s="69"/>
@@ -11930,14 +11586,14 @@
       <c r="A10" s="77" t="s">
         <v>153</v>
       </c>
-      <c r="B10" s="203">
+      <c r="B10" s="197">
         <f>B14/B15 * 4/3 * PI() *B13^3</f>
         <v>5.7453446448850131E-10</v>
       </c>
       <c r="C10" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="D10" s="194" t="s">
+      <c r="D10" s="188" t="s">
         <v>249</v>
       </c>
       <c r="E10" s="69"/>
@@ -11946,14 +11602,14 @@
       <c r="A11" s="77" t="s">
         <v>273</v>
       </c>
-      <c r="B11" s="203">
+      <c r="B11" s="197">
         <f>B10/3</f>
         <v>1.9151148816283376E-10</v>
       </c>
       <c r="C11" s="90" t="s">
         <v>89</v>
       </c>
-      <c r="D11" s="194" t="s">
+      <c r="D11" s="188" t="s">
         <v>274</v>
       </c>
       <c r="E11" s="69"/>
@@ -11962,20 +11618,20 @@
       <c r="A12" s="77" t="s">
         <v>152</v>
       </c>
-      <c r="B12" s="204">
+      <c r="B12" s="198">
         <f>8.3144/1000</f>
         <v>8.3143999999999996E-3</v>
       </c>
       <c r="C12" s="90" t="s">
         <v>222</v>
       </c>
-      <c r="D12" s="194" t="s">
+      <c r="D12" s="188" t="s">
         <v>152</v>
       </c>
       <c r="E12" s="69"/>
     </row>
     <row r="13" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A13" s="170" t="s">
+      <c r="A13" s="169" t="s">
         <v>250</v>
       </c>
       <c r="B13" s="137">
@@ -11984,22 +11640,22 @@
       <c r="C13" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="D13" s="205" t="s">
+      <c r="D13" s="199" t="s">
         <v>251</v>
       </c>
-      <c r="E13" s="229"/>
+      <c r="E13" s="223"/>
     </row>
     <row r="14" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A14" s="77" t="s">
         <v>271</v>
       </c>
-      <c r="B14" s="206">
+      <c r="B14" s="200">
         <v>127</v>
       </c>
       <c r="C14" s="90" t="s">
         <v>252</v>
       </c>
-      <c r="D14" s="207" t="s">
+      <c r="D14" s="201" t="s">
         <v>253</v>
       </c>
       <c r="E14" s="69"/>
@@ -12008,13 +11664,13 @@
       <c r="A15" s="89" t="s">
         <v>272</v>
       </c>
-      <c r="B15" s="208">
+      <c r="B15" s="202">
         <v>25</v>
       </c>
       <c r="C15" s="92" t="s">
         <v>252</v>
       </c>
-      <c r="D15" s="209" t="s">
+      <c r="D15" s="203" t="s">
         <v>254</v>
       </c>
       <c r="E15" s="69"/>
@@ -12045,7 +11701,7 @@
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20"/>
-      <c r="B20" s="185"/>
+      <c r="B20" s="184"/>
       <c r="C20"/>
       <c r="D20"/>
     </row>
@@ -12135,10 +11791,10 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0900-000000000000}">
-  <dimension ref="A1:E10"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12157,7 +11813,7 @@
       <c r="A1" s="77" t="s">
         <v>281</v>
       </c>
-      <c r="B1" s="230">
+      <c r="B1" s="224">
         <f>0.000003997214*0.3</f>
         <v>1.1991642E-6</v>
       </c>
@@ -12167,7 +11823,7 @@
       <c r="D1" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="E1" s="257" t="s">
+      <c r="E1" s="253" t="s">
         <v>164</v>
       </c>
     </row>
@@ -12185,7 +11841,7 @@
       <c r="D2" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="E2" s="258"/>
+      <c r="E2" s="254"/>
     </row>
     <row r="3" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="77" t="s">
@@ -12201,13 +11857,13 @@
       <c r="D3" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="E3" s="258"/>
+      <c r="E3" s="254"/>
     </row>
     <row r="4" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A4" s="77" t="s">
         <v>76</v>
       </c>
-      <c r="B4" s="230">
+      <c r="B4" s="224">
         <f>0.000005457026*0.7</f>
         <v>3.8199181999999996E-6</v>
       </c>
@@ -12217,13 +11873,13 @@
       <c r="D4" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="E4" s="258"/>
+      <c r="E4" s="254"/>
     </row>
     <row r="5" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="77" t="s">
         <v>284</v>
       </c>
-      <c r="B5" s="230">
+      <c r="B5" s="224">
         <f>0.000022716*0.7</f>
         <v>1.5901199999999999E-5</v>
       </c>
@@ -12233,13 +11889,13 @@
       <c r="D5" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="E5" s="258"/>
+      <c r="E5" s="254"/>
     </row>
     <row r="6" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="77" t="s">
         <v>285</v>
       </c>
-      <c r="B6" s="230">
+      <c r="B6" s="224">
         <f>0.000009012152*0.7</f>
         <v>6.3085064000000002E-6</v>
       </c>
@@ -12249,75 +11905,27 @@
       <c r="D6" s="107" t="s">
         <v>163</v>
       </c>
-      <c r="E6" s="258"/>
-    </row>
-    <row r="7" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A7" s="126" t="s">
-        <v>286</v>
-      </c>
-      <c r="B7" s="230">
-        <f>B3</f>
-        <v>5.9220000000000002E-6</v>
-      </c>
-      <c r="C7" s="128" t="s">
-        <v>99</v>
-      </c>
-      <c r="D7" s="193" t="s">
-        <v>163</v>
-      </c>
-      <c r="E7" s="258"/>
-    </row>
-    <row r="8" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A8" s="77" t="s">
-        <v>287</v>
-      </c>
-      <c r="B8" s="230">
-        <f>0.000008892*0.7</f>
-        <v>6.2244000000000001E-6</v>
-      </c>
-      <c r="C8" s="90" t="s">
-        <v>99</v>
-      </c>
-      <c r="D8" s="194" t="s">
-        <v>163</v>
-      </c>
-      <c r="E8" s="258"/>
-    </row>
-    <row r="9" spans="1:5" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A9" s="77" t="s">
-        <v>288</v>
-      </c>
-      <c r="B9" s="230">
-        <f>B5</f>
-        <v>1.5901199999999999E-5</v>
-      </c>
-      <c r="C9" s="90" t="s">
-        <v>99</v>
-      </c>
-      <c r="D9" s="107" t="s">
-        <v>163</v>
-      </c>
-      <c r="E9" s="258"/>
-    </row>
-    <row r="10" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A10" s="89" t="s">
+      <c r="E6" s="254"/>
+    </row>
+    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="89" t="s">
         <v>77</v>
       </c>
-      <c r="B10" s="120">
+      <c r="B7" s="120">
         <f>0.000006143184*0.7</f>
         <v>4.3002288000000002E-6</v>
       </c>
-      <c r="C10" s="92" t="s">
+      <c r="C7" s="92" t="s">
         <v>99</v>
       </c>
-      <c r="D10" s="195" t="s">
+      <c r="D7" s="189" t="s">
         <v>163</v>
       </c>
-      <c r="E10" s="259"/>
+      <c r="E7" s="255"/>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="E1:E10"/>
+    <mergeCell ref="E1:E7"/>
   </mergeCells>
   <conditionalFormatting sqref="E1">
     <cfRule type="expression" dxfId="15" priority="1">
@@ -12352,14 +11960,14 @@
       <c r="A1" s="76" t="s">
         <v>166</v>
       </c>
-      <c r="B1" s="210">
+      <c r="B1" s="204">
         <f>((4/3)*PI()*B3^3)*B4</f>
         <v>2.0943951023931951E-12</v>
       </c>
       <c r="C1" s="91" t="s">
         <v>16</v>
       </c>
-      <c r="D1" s="211" t="s">
+      <c r="D1" s="205" t="s">
         <v>174</v>
       </c>
     </row>
@@ -12374,7 +11982,7 @@
       <c r="C2" s="90" t="s">
         <v>16</v>
       </c>
-      <c r="D2" s="212" t="s">
+      <c r="D2" s="206" t="s">
         <v>175</v>
       </c>
     </row>
@@ -12389,7 +11997,7 @@
       <c r="C3" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="D3" s="212" t="s">
+      <c r="D3" s="206" t="s">
         <v>176</v>
       </c>
     </row>
@@ -12404,7 +12012,7 @@
       <c r="C4" s="90" t="s">
         <v>86</v>
       </c>
-      <c r="D4" s="212" t="s">
+      <c r="D4" s="206" t="s">
         <v>177</v>
       </c>
     </row>
@@ -12419,7 +12027,7 @@
       <c r="C5" s="90" t="s">
         <v>87</v>
       </c>
-      <c r="D5" s="212" t="s">
+      <c r="D5" s="206" t="s">
         <v>178</v>
       </c>
     </row>
@@ -12427,13 +12035,13 @@
       <c r="A6" s="126" t="s">
         <v>198</v>
       </c>
-      <c r="B6" s="180" t="s">
+      <c r="B6" s="179" t="s">
         <v>199</v>
       </c>
       <c r="C6" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="213" t="s">
+      <c r="D6" s="207" t="s">
         <v>255</v>
       </c>
     </row>
@@ -12448,10 +12056,10 @@
       <c r="C7" s="90" t="s">
         <v>85</v>
       </c>
-      <c r="D7" s="212" t="s">
+      <c r="D7" s="206" t="s">
         <v>180</v>
       </c>
-      <c r="E7" s="227"/>
+      <c r="E7" s="221"/>
     </row>
     <row r="8" spans="1:5" ht="28.8" x14ac:dyDescent="0.25">
       <c r="A8" s="77" t="s">
@@ -12464,35 +12072,35 @@
       <c r="C8" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="212" t="s">
+      <c r="D8" s="206" t="s">
         <v>248</v>
       </c>
     </row>
     <row r="9" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A9" s="170" t="s">
+      <c r="A9" s="169" t="s">
         <v>256</v>
       </c>
       <c r="B9" s="122">
         <v>12</v>
       </c>
-      <c r="C9" s="181" t="s">
+      <c r="C9" s="180" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="214" t="s">
+      <c r="D9" s="208" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="26.4" x14ac:dyDescent="0.25">
-      <c r="A10" s="215" t="s">
+      <c r="A10" s="209" t="s">
         <v>258</v>
       </c>
-      <c r="B10" s="182">
+      <c r="B10" s="181">
         <v>12</v>
       </c>
       <c r="C10" s="119" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="216" t="s">
+      <c r="D10" s="210" t="s">
         <v>259</v>
       </c>
     </row>
@@ -12506,7 +12114,7 @@
       <c r="C11" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="212" t="s">
+      <c r="D11" s="206" t="s">
         <v>181</v>
       </c>
     </row>
@@ -12520,7 +12128,7 @@
       <c r="C12" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="212" t="s">
+      <c r="D12" s="206" t="s">
         <v>182</v>
       </c>
     </row>
@@ -12534,7 +12142,7 @@
       <c r="C13" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D13" s="212" t="s">
+      <c r="D13" s="206" t="s">
         <v>184</v>
       </c>
     </row>
@@ -12548,7 +12156,7 @@
       <c r="C14" s="128" t="s">
         <v>88</v>
       </c>
-      <c r="D14" s="213" t="s">
+      <c r="D14" s="207" t="s">
         <v>188</v>
       </c>
     </row>
@@ -12562,7 +12170,7 @@
       <c r="C15" s="90" t="s">
         <v>187</v>
       </c>
-      <c r="D15" s="212" t="s">
+      <c r="D15" s="206" t="s">
         <v>189</v>
       </c>
     </row>
@@ -12570,14 +12178,14 @@
       <c r="A16" s="89" t="s">
         <v>171</v>
       </c>
-      <c r="B16" s="217">
-        <f>800*10^(-6)</f>
-        <v>7.9999999999999993E-4</v>
+      <c r="B16" s="211">
+        <f>400*10^(-6)</f>
+        <v>3.9999999999999996E-4</v>
       </c>
       <c r="C16" s="92" t="s">
         <v>85</v>
       </c>
-      <c r="D16" s="218" t="s">
+      <c r="D16" s="212" t="s">
         <v>179</v>
       </c>
     </row>
@@ -12638,8 +12246,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0A00-000000000000}">
   <dimension ref="A1:D12"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D16" sqref="D16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.44140625" defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12652,13 +12260,13 @@
       <c r="A1" s="76" t="s">
         <v>196</v>
       </c>
-      <c r="B1" s="219">
+      <c r="B1" s="213">
         <v>1E-8</v>
       </c>
       <c r="C1" s="91" t="s">
         <v>79</v>
       </c>
-      <c r="D1" s="211" t="s">
+      <c r="D1" s="205" t="s">
         <v>197</v>
       </c>
     </row>
@@ -12667,12 +12275,12 @@
         <v>200</v>
       </c>
       <c r="B2" s="122" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C2" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D2" s="212" t="s">
+      <c r="D2" s="206" t="s">
         <v>202</v>
       </c>
     </row>
@@ -12686,7 +12294,7 @@
       <c r="C3" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D3" s="212" t="s">
+      <c r="D3" s="206" t="s">
         <v>201</v>
       </c>
     </row>
@@ -12695,12 +12303,12 @@
         <v>229</v>
       </c>
       <c r="B4" s="122" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C4" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D4" s="212" t="s">
+      <c r="D4" s="206" t="s">
         <v>230</v>
       </c>
     </row>
@@ -12714,7 +12322,7 @@
       <c r="C5" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D5" s="212" t="s">
+      <c r="D5" s="206" t="s">
         <v>235</v>
       </c>
     </row>
@@ -12728,7 +12336,7 @@
       <c r="C6" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D6" s="212" t="s">
+      <c r="D6" s="206" t="s">
         <v>205</v>
       </c>
     </row>
@@ -12736,13 +12344,13 @@
       <c r="A7" s="77" t="s">
         <v>190</v>
       </c>
-      <c r="B7" s="183">
+      <c r="B7" s="182">
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="C7" s="90" t="s">
         <v>261</v>
       </c>
-      <c r="D7" s="212" t="s">
+      <c r="D7" s="206" t="s">
         <v>262</v>
       </c>
     </row>
@@ -12756,7 +12364,7 @@
       <c r="C8" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D8" s="212" t="s">
+      <c r="D8" s="206" t="s">
         <v>195</v>
       </c>
     </row>
@@ -12770,7 +12378,7 @@
       <c r="C9" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D9" s="212" t="s">
+      <c r="D9" s="206" t="s">
         <v>194</v>
       </c>
     </row>
@@ -12778,13 +12386,13 @@
       <c r="A10" s="105" t="s">
         <v>206</v>
       </c>
-      <c r="B10" s="179" t="b">
+      <c r="B10" s="178" t="b">
         <v>0</v>
       </c>
       <c r="C10" s="119" t="s">
         <v>88</v>
       </c>
-      <c r="D10" s="220" t="s">
+      <c r="D10" s="214" t="s">
         <v>207</v>
       </c>
     </row>
@@ -12798,7 +12406,7 @@
       <c r="C11" s="90" t="s">
         <v>88</v>
       </c>
-      <c r="D11" s="205" t="s">
+      <c r="D11" s="199" t="s">
         <v>233</v>
       </c>
     </row>
@@ -12806,13 +12414,13 @@
       <c r="A12" s="89" t="s">
         <v>231</v>
       </c>
-      <c r="B12" s="221" t="s">
+      <c r="B12" s="215" t="s">
         <v>100</v>
       </c>
       <c r="C12" s="92" t="s">
         <v>88</v>
       </c>
-      <c r="D12" s="222" t="s">
+      <c r="D12" s="216" t="s">
         <v>234</v>
       </c>
     </row>

</xml_diff>